<commit_message>
feat: update CMBS categorization and use dynamic attribution values from Excel
</commit_message>
<xml_diff>
--- a/data/Risk Report Format Master Sheet.xlsx
+++ b/data/Risk Report Format Master Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BW Code\BD Script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73F8A5D-D0D9-4A75-8A08-0F331FAE7D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{0D00A85A-72D1-472E-B2C5-9380F1294116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="4110" windowWidth="43200" windowHeight="23220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key Stats" sheetId="10" r:id="rId1"/>
@@ -24,6 +24,7 @@
   <pivotCaches>
     <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="214">
   <si>
     <t>CMBS F1</t>
   </si>
@@ -2838,19 +2839,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.74184585080773002</c:v>
+                  <c:v>0.70595795072435885</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14052368340793228</c:v>
+                  <c:v>0.14321007890326481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6246288637051309E-2</c:v>
+                  <c:v>1.6419670822658293E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6188003814129888E-2</c:v>
+                  <c:v>9.3025797079759651E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0547925554549654E-3</c:v>
+                  <c:v>7.1859815159926697E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3367,13 +3368,13 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.52300000000000002</c:v>
+                  <c:v>0.4824</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.6000000000000001E-2</c:v>
+                  <c:v>4.8599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27200000000000002</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.14799999999999999</c:v>
@@ -6243,607 +6244,607 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="201"/>
                 <c:pt idx="0">
-                  <c:v>2.7538990223589292E-2</c:v>
+                  <c:v>2.7045167236918379E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6175154413272166E-2</c:v>
+                  <c:v>2.3904760962183986E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3464186653468201E-2</c:v>
+                  <c:v>2.1603660596083377E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0811674921631201E-2</c:v>
+                  <c:v>1.9924891708791987E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9578768201385599E-2</c:v>
+                  <c:v>1.8795128400195395E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.8773493030693669E-2</c:v>
+                  <c:v>1.8136468756324804E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7809812530165472E-2</c:v>
+                  <c:v>1.7927162195716238E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7383613835201994E-2</c:v>
+                  <c:v>1.7747018684793562E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7184630522191321E-2</c:v>
+                  <c:v>1.7329283087763811E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5794804338968228E-2</c:v>
+                  <c:v>1.6245822084007003E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4686433846166231E-2</c:v>
+                  <c:v>1.6215952440089339E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.449786664032068E-2</c:v>
+                  <c:v>1.4966974253448648E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.4409305989080376E-2</c:v>
+                  <c:v>1.4755062591656685E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4404284098204045E-2</c:v>
+                  <c:v>1.4601423232270183E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.3648127397534097E-2</c:v>
+                  <c:v>1.4407109514828931E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.3559905308638615E-2</c:v>
+                  <c:v>1.400765392540677E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.3551353397569917E-2</c:v>
+                  <c:v>1.3808527746987919E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.3545218864184213E-2</c:v>
+                  <c:v>1.3785320492214644E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3260831776829964E-2</c:v>
+                  <c:v>1.3782696492379233E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3045521512526304E-2</c:v>
+                  <c:v>1.3316895963347531E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2992104519820752E-2</c:v>
+                  <c:v>1.3290563984191131E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2952178621811184E-2</c:v>
+                  <c:v>1.3290102202738616E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2944305298576649E-2</c:v>
+                  <c:v>1.3154691649279415E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2746180150098659E-2</c:v>
+                  <c:v>1.24889344917126E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2201966476852724E-2</c:v>
+                  <c:v>1.2457824356290255E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2127343849557545E-2</c:v>
+                  <c:v>1.2452337038115928E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.2004386987440666E-2</c:v>
+                  <c:v>1.2344434418284821E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.1400472902684712E-2</c:v>
+                  <c:v>1.1674234227663366E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1101553557256413E-2</c:v>
+                  <c:v>1.1313987087633696E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.1071060939994787E-2</c:v>
+                  <c:v>1.1295592404275722E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.088437447963592E-2</c:v>
+                  <c:v>1.1087344540907146E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.0571910778369747E-2</c:v>
+                  <c:v>1.0844735656461549E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.0486020124955267E-2</c:v>
+                  <c:v>1.0837174856599104E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.0290284203770549E-2</c:v>
+                  <c:v>1.0813252683352153E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0147863308924242E-2</c:v>
+                  <c:v>1.0436510926848695E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.0017902508887424E-2</c:v>
+                  <c:v>1.0355471201628901E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.6768736269436818E-3</c:v>
+                  <c:v>1.0336396539525701E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.6377781494518429E-3</c:v>
+                  <c:v>9.9635364336205165E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.3896733693005566E-3</c:v>
+                  <c:v>9.6009794199983598E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.3418450702200135E-3</c:v>
+                  <c:v>9.5581465570284962E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.0548278345516531E-3</c:v>
+                  <c:v>9.5418652509790397E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>8.8717789268286575E-3</c:v>
+                  <c:v>9.0132674831253663E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>8.6618696394714645E-3</c:v>
+                  <c:v>8.9809918986178735E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.6058060203857388E-3</c:v>
+                  <c:v>8.9695553703790041E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8.5170073349799397E-3</c:v>
+                  <c:v>8.8735299252237741E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.4545708958043697E-3</c:v>
+                  <c:v>8.830250797298737E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8.2135133901149286E-3</c:v>
+                  <c:v>8.8113767176745388E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>8.0682192187579681E-3</c:v>
+                  <c:v>8.5541157455958083E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7.9825308419737961E-3</c:v>
+                  <c:v>8.3886403495779891E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7.9637372411657734E-3</c:v>
+                  <c:v>8.3736105788035642E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.9136900695474868E-3</c:v>
+                  <c:v>8.1142680768890689E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7.883877425358574E-3</c:v>
+                  <c:v>8.1068374830790598E-3</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7.7163517793967353E-3</c:v>
+                  <c:v>8.0098082282224828E-3</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7.6751519147574545E-3</c:v>
+                  <c:v>7.8078792513262404E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7.5514212571688158E-3</c:v>
+                  <c:v>7.7291554461632016E-3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7.4724118813838964E-3</c:v>
+                  <c:v>7.6446839245256715E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7.4122524951454353E-3</c:v>
+                  <c:v>7.5549132567558856E-3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7.3294935411766828E-3</c:v>
+                  <c:v>7.4397410750912021E-3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7.2687594965938187E-3</c:v>
+                  <c:v>7.439224005763365E-3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.8481960801705143E-3</c:v>
+                  <c:v>7.4173665206023953E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.8370576896229114E-3</c:v>
+                  <c:v>7.302752836209076E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6.731083246290904E-3</c:v>
+                  <c:v>7.2060601540586602E-3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>6.6698221792003123E-3</c:v>
+                  <c:v>7.0279479790355051E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.6071639813753379E-3</c:v>
+                  <c:v>6.9409638201818448E-3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.5822842029454173E-3</c:v>
+                  <c:v>6.8403963069613482E-3</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.5208647937831932E-3</c:v>
+                  <c:v>6.7237767149497417E-3</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>6.4987666602881302E-3</c:v>
+                  <c:v>6.6724867121063141E-3</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>6.3058261481941727E-3</c:v>
+                  <c:v>6.6718843296525157E-3</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>6.1963349339672572E-3</c:v>
+                  <c:v>6.603022666631814E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.0920297455003443E-3</c:v>
+                  <c:v>6.3044161513552488E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6.0099686825839521E-3</c:v>
+                  <c:v>6.23035426677521E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.8800514446850586E-3</c:v>
+                  <c:v>6.1379660873850973E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5.8381302673505674E-3</c:v>
+                  <c:v>5.4219477370113338E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5.7261858380325964E-3</c:v>
+                  <c:v>5.356228620258161E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>5.2766908387614966E-3</c:v>
+                  <c:v>5.3309906093833093E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5.2595503270582442E-3</c:v>
+                  <c:v>5.304312546073533E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.2365108958190741E-3</c:v>
+                  <c:v>5.2854903721699835E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.2364779439928412E-3</c:v>
+                  <c:v>5.165855444320579E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.1467129096084219E-3</c:v>
+                  <c:v>5.0715470293606771E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.0749588942454312E-3</c:v>
+                  <c:v>4.9086085806584745E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.8906189761698743E-3</c:v>
+                  <c:v>4.8661613109304176E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.8822368329879337E-3</c:v>
+                  <c:v>4.7596380442114427E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.7936650182820858E-3</c:v>
+                  <c:v>4.6736227001118276E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.7287124143296968E-3</c:v>
+                  <c:v>4.6391174750034488E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.6244217380966707E-3</c:v>
+                  <c:v>4.5528456807515695E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.4780158971009891E-3</c:v>
+                  <c:v>4.349327477692384E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.3730006228254832E-3</c:v>
+                  <c:v>4.1292133729805783E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.2492448862754516E-3</c:v>
+                  <c:v>4.0444672894074099E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.2258105687921496E-3</c:v>
+                  <c:v>3.9105062446114971E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.0224209274573562E-3</c:v>
+                  <c:v>3.9062833691188023E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>3.9982923929708222E-3</c:v>
+                  <c:v>3.8940015783066888E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3.9638300281556373E-3</c:v>
+                  <c:v>3.8812537817998999E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>3.9200268048395666E-3</c:v>
+                  <c:v>3.7128962654241413E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>3.8416751225075038E-3</c:v>
+                  <c:v>3.4870783846391302E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>3.8084889614445755E-3</c:v>
+                  <c:v>3.3992419228086267E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.8074484716491843E-3</c:v>
+                  <c:v>3.361303313740524E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>3.7633254550290323E-3</c:v>
+                  <c:v>3.3140140961680315E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>3.6072805072487231E-3</c:v>
+                  <c:v>3.182964230650794E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.3347110225668336E-3</c:v>
+                  <c:v>3.1654316792252757E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3.3214781128092911E-3</c:v>
+                  <c:v>3.1492288253594479E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>3.2176313684901714E-3</c:v>
+                  <c:v>3.1384277556665775E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>3.1626201442374788E-3</c:v>
+                  <c:v>2.7676953701666518E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>3.0944504455674097E-3</c:v>
+                  <c:v>2.757823827014803E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>3.0823578746581671E-3</c:v>
+                  <c:v>2.7097665566285342E-3</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.8134838196032202E-3</c:v>
+                  <c:v>2.6941034532339016E-3</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.713956163343037E-3</c:v>
+                  <c:v>2.5378013717921978E-3</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.6796669280809674E-3</c:v>
+                  <c:v>2.4922277625296025E-3</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2.6510986745924962E-3</c:v>
+                  <c:v>2.277405956812435E-3</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.6461835949039068E-3</c:v>
+                  <c:v>2.174031821209062E-3</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.5477842639907771E-3</c:v>
+                  <c:v>2.1326922140377895E-3</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.4011727169126291E-3</c:v>
+                  <c:v>2.0481472237179996E-3</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.2970995308723443E-3</c:v>
+                  <c:v>1.9358285452413314E-3</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.1804501521514677E-3</c:v>
+                  <c:v>1.8483333359146758E-3</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.1525158010601043E-3</c:v>
+                  <c:v>1.781638833364099E-3</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>2.0749072330865175E-3</c:v>
+                  <c:v>1.6988457025303829E-3</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>2.0697183143433217E-3</c:v>
+                  <c:v>1.683440070836772E-3</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1.9060237075932489E-3</c:v>
+                  <c:v>1.6212380774320108E-3</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>1.8005989181893109E-3</c:v>
+                  <c:v>1.5699138527052079E-3</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1.7795385160118196E-3</c:v>
+                  <c:v>1.4205367674621286E-3</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>1.6451045493905145E-3</c:v>
+                  <c:v>1.3766998463060867E-3</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1.6021119865575009E-3</c:v>
+                  <c:v>1.229614785161664E-3</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>1.3665707949721002E-3</c:v>
+                  <c:v>1.2096244012303806E-3</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>1.2334755881539413E-3</c:v>
+                  <c:v>1.1809214350173135E-3</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1.2161443569352075E-3</c:v>
+                  <c:v>1.1655820659458092E-3</c:v>
                 </c:pt>
                 <c:pt idx="124" formatCode="0.00">
-                  <c:v>1.1845293656542976E-3</c:v>
+                  <c:v>1.1232624345935847E-3</c:v>
                 </c:pt>
                 <c:pt idx="125" formatCode="0.00">
-                  <c:v>1.1834435138390112E-3</c:v>
+                  <c:v>1.0399113448723081E-3</c:v>
                 </c:pt>
                 <c:pt idx="126" formatCode="0.00">
-                  <c:v>1.1508091723830057E-3</c:v>
+                  <c:v>1.0097024777435978E-3</c:v>
                 </c:pt>
                 <c:pt idx="127" formatCode="0.00">
-                  <c:v>1.0159195761445207E-3</c:v>
+                  <c:v>9.0792819793212903E-4</c:v>
                 </c:pt>
                 <c:pt idx="128" formatCode="0.00">
-                  <c:v>9.8710701607583932E-4</c:v>
+                  <c:v>9.0571893308754074E-4</c:v>
                 </c:pt>
                 <c:pt idx="129" formatCode="General">
-                  <c:v>9.7776974515775719E-4</c:v>
+                  <c:v>6.9754948048845664E-4</c:v>
                 </c:pt>
                 <c:pt idx="130" formatCode="General">
-                  <c:v>8.7743970954118171E-4</c:v>
+                  <c:v>6.2843659930169411E-4</c:v>
                 </c:pt>
                 <c:pt idx="131" formatCode="General">
-                  <c:v>6.8705800341977645E-4</c:v>
+                  <c:v>6.1893963323072696E-4</c:v>
                 </c:pt>
                 <c:pt idx="132" formatCode="General">
-                  <c:v>6.1098114967575695E-4</c:v>
+                  <c:v>5.6421619120872331E-4</c:v>
                 </c:pt>
                 <c:pt idx="133" formatCode="General">
-                  <c:v>6.0880109383079509E-4</c:v>
+                  <c:v>5.3032487548944688E-4</c:v>
                 </c:pt>
                 <c:pt idx="134" formatCode="General">
-                  <c:v>5.8470717445661046E-4</c:v>
+                  <c:v>5.0428471415985953E-4</c:v>
                 </c:pt>
                 <c:pt idx="135" formatCode="General">
-                  <c:v>5.4172516658072584E-4</c:v>
+                  <c:v>4.5711648109156289E-4</c:v>
                 </c:pt>
                 <c:pt idx="136" formatCode="General">
-                  <c:v>5.1475863032430288E-4</c:v>
+                  <c:v>4.3247129980915529E-4</c:v>
                 </c:pt>
                 <c:pt idx="137" formatCode="General">
-                  <c:v>4.4944863583792422E-4</c:v>
+                  <c:v>3.9178183939844903E-4</c:v>
                 </c:pt>
                 <c:pt idx="138" formatCode="General">
-                  <c:v>4.4929766848566936E-4</c:v>
+                  <c:v>3.6420198321594457E-4</c:v>
                 </c:pt>
                 <c:pt idx="139" formatCode="General">
-                  <c:v>4.1196543597449579E-4</c:v>
+                  <c:v>3.6417325560831888E-4</c:v>
                 </c:pt>
                 <c:pt idx="140" formatCode="General">
-                  <c:v>4.0713183969113583E-4</c:v>
+                  <c:v>3.58466373474702E-4</c:v>
                 </c:pt>
                 <c:pt idx="141" formatCode="General">
-                  <c:v>3.9384740829201848E-4</c:v>
+                  <c:v>3.1853974769628147E-4</c:v>
                 </c:pt>
                 <c:pt idx="142" formatCode="General">
-                  <c:v>3.4211302945093345E-4</c:v>
+                  <c:v>2.898317151535657E-4</c:v>
                 </c:pt>
                 <c:pt idx="143" formatCode="General">
-                  <c:v>3.1919983680591622E-4</c:v>
+                  <c:v>2.530936329461867E-4</c:v>
                 </c:pt>
                 <c:pt idx="144" formatCode="General">
-                  <c:v>2.7370125900597514E-4</c:v>
+                  <c:v>2.4822193594536778E-4</c:v>
                 </c:pt>
                 <c:pt idx="145" formatCode="General">
-                  <c:v>2.6350839084243922E-4</c:v>
+                  <c:v>2.4632715626623857E-4</c:v>
                 </c:pt>
                 <c:pt idx="146" formatCode="General">
-                  <c:v>2.5486115427478213E-4</c:v>
+                  <c:v>2.3683473194582833E-4</c:v>
                 </c:pt>
                 <c:pt idx="147" formatCode="General">
-                  <c:v>2.5108296897734505E-4</c:v>
+                  <c:v>2.3627415016280918E-4</c:v>
                 </c:pt>
                 <c:pt idx="148" formatCode="General">
-                  <c:v>2.4256813271656685E-4</c:v>
+                  <c:v>2.2131391372745638E-4</c:v>
                 </c:pt>
                 <c:pt idx="149" formatCode="General">
-                  <c:v>2.2142519471729996E-4</c:v>
+                  <c:v>1.8839599592692126E-4</c:v>
                 </c:pt>
                 <c:pt idx="150" formatCode="General">
-                  <c:v>2.1357628362057244E-4</c:v>
+                  <c:v>1.8744844043080134E-4</c:v>
                 </c:pt>
                 <c:pt idx="151" formatCode="General">
-                  <c:v>2.0004548913559538E-4</c:v>
+                  <c:v>1.7840391002169084E-4</c:v>
                 </c:pt>
                 <c:pt idx="152" formatCode="General">
-                  <c:v>1.9897338344245028E-4</c:v>
+                  <c:v>1.7208811580505601E-4</c:v>
                 </c:pt>
                 <c:pt idx="153" formatCode="General">
-                  <c:v>1.9333374608214679E-4</c:v>
+                  <c:v>1.4819373144525148E-4</c:v>
                 </c:pt>
                 <c:pt idx="154" formatCode="General">
-                  <c:v>1.8282883540970011E-4</c:v>
+                  <c:v>1.3688568366970313E-4</c:v>
                 </c:pt>
                 <c:pt idx="155" formatCode="General">
-                  <c:v>1.4719652638100125E-4</c:v>
+                  <c:v>1.3560021641026706E-4</c:v>
                 </c:pt>
                 <c:pt idx="156" formatCode="General">
-                  <c:v>1.4025003909898376E-4</c:v>
+                  <c:v>1.3450779425656727E-4</c:v>
                 </c:pt>
                 <c:pt idx="157" formatCode="General">
-                  <c:v>1.3996543887037646E-4</c:v>
+                  <c:v>1.33467830012035E-4</c:v>
                 </c:pt>
                 <c:pt idx="158" formatCode="General">
-                  <c:v>1.3730853781448554E-4</c:v>
+                  <c:v>1.3151123282836575E-4</c:v>
                 </c:pt>
                 <c:pt idx="159" formatCode="General">
-                  <c:v>1.3502430368333087E-4</c:v>
+                  <c:v>1.2711458360919719E-4</c:v>
                 </c:pt>
                 <c:pt idx="160" formatCode="General">
-                  <c:v>1.2915618166881306E-4</c:v>
+                  <c:v>1.1960070596602893E-4</c:v>
                 </c:pt>
                 <c:pt idx="161" formatCode="General">
-                  <c:v>1.2416608113498395E-4</c:v>
+                  <c:v>1.1331136157938487E-4</c:v>
                 </c:pt>
                 <c:pt idx="162" formatCode="General">
-                  <c:v>1.236892848004802E-4</c:v>
+                  <c:v>1.0651080106319081E-4</c:v>
                 </c:pt>
                 <c:pt idx="163" formatCode="General">
-                  <c:v>1.1004579644682239E-4</c:v>
+                  <c:v>1.0268093194315097E-4</c:v>
                 </c:pt>
                 <c:pt idx="164" formatCode="General">
-                  <c:v>1.0686869744400136E-4</c:v>
+                  <c:v>8.9365112913069217E-5</c:v>
                 </c:pt>
                 <c:pt idx="165" formatCode="General">
-                  <c:v>1.0489848001900734E-4</c:v>
+                  <c:v>7.0192975731807981E-5</c:v>
                 </c:pt>
                 <c:pt idx="166" formatCode="General">
-                  <c:v>1.0443373857403633E-4</c:v>
+                  <c:v>6.6937424084161424E-5</c:v>
                 </c:pt>
                 <c:pt idx="167" formatCode="General">
-                  <c:v>7.1963977090625574E-5</c:v>
+                  <c:v>6.4427754881311701E-5</c:v>
                 </c:pt>
                 <c:pt idx="168" formatCode="General">
-                  <c:v>7.1029331197009651E-5</c:v>
+                  <c:v>6.3388025316899371E-5</c:v>
                 </c:pt>
                 <c:pt idx="169" formatCode="General">
-                  <c:v>6.9025732300064416E-5</c:v>
+                  <c:v>6.2095020684198706E-5</c:v>
                 </c:pt>
                 <c:pt idx="170" formatCode="General">
-                  <c:v>6.6173303165213058E-5</c:v>
+                  <c:v>5.9397193243992999E-5</c:v>
                 </c:pt>
                 <c:pt idx="171" formatCode="General">
-                  <c:v>5.5899340786949375E-5</c:v>
+                  <c:v>5.356010505793728E-5</c:v>
                 </c:pt>
                 <c:pt idx="172" formatCode="General">
-                  <c:v>5.1785610338711489E-5</c:v>
+                  <c:v>5.1749478908883005E-5</c:v>
                 </c:pt>
                 <c:pt idx="173" formatCode="General">
-                  <c:v>5.1568403245883209E-5</c:v>
+                  <c:v>4.8023227964161854E-5</c:v>
                 </c:pt>
                 <c:pt idx="174" formatCode="General">
-                  <c:v>4.9573788584415942E-5</c:v>
+                  <c:v>4.63298866562357E-5</c:v>
                 </c:pt>
                 <c:pt idx="175" formatCode="General">
-                  <c:v>4.8646941919557083E-5</c:v>
+                  <c:v>4.5385533853517606E-5</c:v>
                 </c:pt>
                 <c:pt idx="176" formatCode="General">
-                  <c:v>4.4789283016749116E-5</c:v>
+                  <c:v>4.2419922591724881E-5</c:v>
                 </c:pt>
                 <c:pt idx="177" formatCode="General">
-                  <c:v>4.3537711182550642E-5</c:v>
+                  <c:v>4.0612982301025267E-5</c:v>
                 </c:pt>
                 <c:pt idx="178" formatCode="General">
-                  <c:v>4.1990928478682653E-5</c:v>
+                  <c:v>3.9335797869352471E-5</c:v>
                 </c:pt>
                 <c:pt idx="179" formatCode="General">
-                  <c:v>4.021427606369372E-5</c:v>
+                  <c:v>3.4469401878302092E-5</c:v>
                 </c:pt>
                 <c:pt idx="180" formatCode="General">
-                  <c:v>3.57033970489855E-5</c:v>
+                  <c:v>3.1090367073417888E-5</c:v>
                 </c:pt>
                 <c:pt idx="181" formatCode="General">
-                  <c:v>3.3837379770206766E-5</c:v>
+                  <c:v>2.389260355183545E-5</c:v>
                 </c:pt>
                 <c:pt idx="182" formatCode="General">
-                  <c:v>3.3168590878083439E-5</c:v>
+                  <c:v>2.3589990439503803E-5</c:v>
                 </c:pt>
                 <c:pt idx="183" formatCode="General">
-                  <c:v>2.9786196238130884E-5</c:v>
+                  <c:v>2.200511276113788E-5</c:v>
                 </c:pt>
                 <c:pt idx="184" formatCode="General">
-                  <c:v>2.9487795618432913E-5</c:v>
+                  <c:v>1.4673995712566542E-5</c:v>
                 </c:pt>
                 <c:pt idx="185" formatCode="General">
-                  <c:v>2.8565519387390181E-5</c:v>
+                  <c:v>1.4291991696123799E-5</c:v>
                 </c:pt>
                 <c:pt idx="186" formatCode="General">
-                  <c:v>2.7905045311209616E-5</c:v>
+                  <c:v>1.3819580614644794E-5</c:v>
                 </c:pt>
                 <c:pt idx="187" formatCode="General">
-                  <c:v>1.5594980626555879E-5</c:v>
+                  <c:v>1.2170345364558136E-5</c:v>
                 </c:pt>
                 <c:pt idx="188" formatCode="General">
-                  <c:v>1.5388713080254792E-5</c:v>
+                  <c:v>1.2163581055218121E-5</c:v>
                 </c:pt>
                 <c:pt idx="189" formatCode="General">
-                  <c:v>1.3863069748482871E-5</c:v>
+                  <c:v>1.2038689817260709E-5</c:v>
                 </c:pt>
                 <c:pt idx="190" formatCode="General">
-                  <c:v>1.2997503375131399E-5</c:v>
+                  <c:v>9.7038434990680698E-6</c:v>
                 </c:pt>
                 <c:pt idx="191" formatCode="General">
-                  <c:v>1.1391878332580339E-5</c:v>
+                  <c:v>8.1843173317544709E-6</c:v>
                 </c:pt>
                 <c:pt idx="192" formatCode="General">
-                  <c:v>8.6902776151212632E-6</c:v>
+                  <c:v>7.8843823337329525E-6</c:v>
                 </c:pt>
                 <c:pt idx="193" formatCode="General">
-                  <c:v>8.6404873402441047E-6</c:v>
+                  <c:v>3.55989034909555E-6</c:v>
                 </c:pt>
                 <c:pt idx="194" formatCode="General">
-                  <c:v>6.4933118760205351E-6</c:v>
+                  <c:v>3.4667085367585843E-6</c:v>
                 </c:pt>
                 <c:pt idx="195" formatCode="General">
-                  <c:v>5.8556448531297556E-6</c:v>
+                  <c:v>1.1336706359609298E-6</c:v>
                 </c:pt>
                 <c:pt idx="196" formatCode="General">
-                  <c:v>4.6376463397207115E-6</c:v>
+                  <c:v>1.0780376428175266E-6</c:v>
                 </c:pt>
                 <c:pt idx="197" formatCode="General">
-                  <c:v>1.3789169055860547E-6</c:v>
+                  <c:v>3.6449964043633121E-7</c:v>
                 </c:pt>
                 <c:pt idx="198" formatCode="General">
-                  <c:v>1.2717519723324345E-6</c:v>
+                  <c:v>2.9464779296595409E-7</c:v>
                 </c:pt>
                 <c:pt idx="199" formatCode="General">
-                  <c:v>4.8482166681834344E-7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="200" formatCode="General">
-                  <c:v>3.3178941186481388E-7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8921,25 +8922,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0" formatCode="0.00%">
-                  <c:v>1.54E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00%">
-                  <c:v>4.8999999999999998E-3</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00%">
-                  <c:v>-6.9999999999999999E-4</c:v>
+                  <c:v>-5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00%">
-                  <c:v>2.0000000000000001E-4</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00%">
                   <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00%">
-                  <c:v>2.01E-2</c:v>
+                  <c:v>9.2999999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00%">
-                  <c:v>1.49E-2</c:v>
+                  <c:v>6.3E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9178,8 +9179,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.175446031275067E-3"/>
-                  <c:y val="2.94413008017014E-2"/>
+                  <c:x val="-0.14490046811687274"/>
+                  <c:y val="2.2082569152896931E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -9319,19 +9320,19 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="1">
-                  <c:v>6.7999999999999996E-3</c:v>
+                  <c:v>6.1000000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.1000000000000004E-3</c:v>
+                  <c:v>6.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.1999999999999998E-3</c:v>
+                  <c:v>-3.2000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.01E-2</c:v>
+                  <c:v>9.300000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.49E-2</c:v>
+                  <c:v>6.3E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9919,25 +9920,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0" formatCode="0.00%">
-                  <c:v>1.54E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00%">
-                  <c:v>4.8999999999999998E-3</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00%">
-                  <c:v>-6.9999999999999999E-4</c:v>
+                  <c:v>-5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0.00%">
-                  <c:v>2.0000000000000001E-4</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00%">
                   <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00%">
-                  <c:v>2.01E-2</c:v>
+                  <c:v>9.2999999999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00%">
-                  <c:v>1.49E-2</c:v>
+                  <c:v>6.3E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20122,16 +20123,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>278</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>308</xdr:row>
-      <xdr:rowOff>91168</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>408214</xdr:colOff>
+      <xdr:row>306</xdr:row>
+      <xdr:rowOff>91169</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20421,7 +20422,7 @@
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>%  | $3.667mm</a:t>
+            <a:t>%  | $3.6mm</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -20464,7 +20465,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>179</a:t>
+            <a:t>177</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -20490,7 +20491,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>19</a:t>
+            <a:t>21</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -20508,7 +20509,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>: 3</a:t>
+            <a:t>: 4</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1600" i="0" baseline="0">
             <a:solidFill>
@@ -21258,7 +21259,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -21281,7 +21282,8 @@
         <v>206</v>
       </c>
       <c r="B2" s="215">
-        <v>5.4999999999999997E-3</v>
+        <f>'Credit Risk Tables'!AP52</f>
+        <v>6.3E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -21297,7 +21299,8 @@
         <v>208</v>
       </c>
       <c r="B4" s="292">
-        <v>737470611</v>
+        <f>'Credit Risk Tables'!J4*1000000</f>
+        <v>742903999.99999988</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -21306,7 +21309,7 @@
       </c>
       <c r="B6" s="215">
         <f>'Credit Risk Tables'!BP58</f>
-        <v>0.13800000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -21315,7 +21318,7 @@
       </c>
       <c r="B7" s="253">
         <f>'Credit Risk Tables'!BP59</f>
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -21333,7 +21336,7 @@
       </c>
       <c r="B9" s="3">
         <f>'Credit Risk Tables'!Q4</f>
-        <v>0.1939082414860159</v>
+        <v>0.16558995720480763</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -21342,7 +21345,7 @@
       </c>
       <c r="B10" s="3">
         <f>'Postion Level'!C282</f>
-        <v>0.52300000000000002</v>
+        <v>0.4824</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -21351,7 +21354,7 @@
       </c>
       <c r="B11" s="215">
         <f>'Credit Risk Tables'!S16</f>
-        <v>6.6835595270179678E-3</v>
+        <v>6.0317349213357321E-3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -21360,7 +21363,7 @@
       </c>
       <c r="B12" s="291">
         <f>'Credit Risk Tables'!K4</f>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -21378,7 +21381,7 @@
       </c>
       <c r="B14" s="291">
         <f>'Credit Risk Tables'!K6</f>
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -21387,7 +21390,7 @@
       </c>
       <c r="B15" s="291">
         <f>'Credit Risk Tables'!K7</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -21404,7 +21407,7 @@
       </c>
       <c r="B17" s="215">
         <f>SUM('Postion Level'!B2:B11)</f>
-        <v>0.20451512867056715</v>
+        <v>0.19865936371277854</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -21413,7 +21416,7 @@
       </c>
       <c r="B18" s="215">
         <f>'Credit Risk Tables'!AM82</f>
-        <v>0.12347046706366238</v>
+        <v>0.13327832398264117</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -21422,7 +21425,7 @@
       </c>
       <c r="B19" s="293">
         <f>'Credit Risk Tables'!AM74</f>
-        <v>-79.911000000000001</v>
+        <v>-87.734999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -21435,7 +21438,7 @@
       </c>
       <c r="B22" s="215">
         <f>'Credit Risk Tables'!AP35</f>
-        <v>1.54E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -21445,7 +21448,7 @@
       </c>
       <c r="B23" s="215">
         <f>'Credit Risk Tables'!AP38</f>
-        <v>4.8999999999999998E-3</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -21455,7 +21458,7 @@
       </c>
       <c r="B24" s="215">
         <f>'Credit Risk Tables'!AP43</f>
-        <v>2.0000000000000001E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -21465,7 +21468,7 @@
       </c>
       <c r="B25" s="215">
         <f>'Credit Risk Tables'!AP41</f>
-        <v>-6.9999999999999999E-4</v>
+        <v>-5.9999999999999995E-4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -21485,7 +21488,7 @@
       </c>
       <c r="B27" s="215">
         <f>'Credit Risk Tables'!AP49</f>
-        <v>2.01E-2</v>
+        <v>9.2999999999999992E-3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -21495,7 +21498,7 @@
       </c>
       <c r="B28" s="215">
         <f>'Credit Risk Tables'!AP52</f>
-        <v>1.49E-2</v>
+        <v>6.3E-3</v>
       </c>
     </row>
   </sheetData>
@@ -21509,7 +21512,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -21685,10 +21688,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C87F62-F0F0-45CB-BB72-416411A41A89}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="B1:BU145"/>
+  <dimension ref="B1:BU154"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:Q12"/>
+    <sheetView topLeftCell="AA12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL73" sqref="AL73:AM82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21850,61 +21853,61 @@
     <row r="4" spans="2:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <f>F4/J4</f>
-        <v>1.1234704670636624</v>
+        <v>1.1332783239826412</v>
       </c>
       <c r="D4" s="53">
         <f>J4-H4-I4</f>
-        <v>829.49899999999991</v>
+        <v>841.84499999999991</v>
       </c>
       <c r="E4" s="223" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="264">
         <f>SUM(F5:F10)</f>
-        <v>829.54699999999991</v>
+        <v>841.91699999999992</v>
       </c>
       <c r="G4" s="265">
         <f>SUM(G5:G10)</f>
-        <v>-4.8000000000000001E-2</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="H4" s="265">
         <f>SUM(H5:H8)</f>
-        <v>-79.911000000000001</v>
+        <v>-87.734999999999999</v>
       </c>
       <c r="I4" s="265">
         <f>I5+I6</f>
-        <v>-11.209</v>
+        <v>-11.206</v>
       </c>
       <c r="J4" s="264">
         <f>SUM(J5:J10)</f>
-        <v>738.37899999999991</v>
+        <v>742.90399999999988</v>
       </c>
       <c r="K4" s="105">
         <f>SUM(K5:K10)</f>
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L4" s="265">
         <f>SUM(L5:L10)</f>
-        <v>80239</v>
+        <v>61916</v>
       </c>
       <c r="M4" s="265">
         <f>SUM(M5:M10)</f>
-        <v>63449.295127040154</v>
+        <v>67627.888410688494</v>
       </c>
       <c r="N4" s="267">
-        <v>78.2</v>
+        <v>77.47</v>
       </c>
       <c r="O4" s="265">
         <f>SUM(O5:O10)</f>
-        <v>4.9349999999999996</v>
+        <v>4.4809999999999999</v>
       </c>
       <c r="P4" s="45">
         <f>100%-C34</f>
-        <v>0.9813970874036233</v>
+        <v>0.98169346241237088</v>
       </c>
       <c r="Q4" s="268">
         <f>B18</f>
-        <v>0.1939082414860159</v>
+        <v>0.16558995720480763</v>
       </c>
       <c r="R4" s="91">
         <v>0.214</v>
@@ -21929,42 +21932,42 @@
     <row r="5" spans="2:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D5" s="82">
         <f>F5/F4</f>
-        <v>0.14052368340793228</v>
+        <v>0.14321007890326481</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="263">
         <f>J5-H5-I5</f>
-        <v>116.571</v>
+        <v>120.571</v>
       </c>
       <c r="G5" s="40">
         <v>0</v>
       </c>
       <c r="H5" s="40">
-        <v>-13.887</v>
+        <v>-23.619</v>
       </c>
       <c r="I5" s="40">
         <v>0</v>
       </c>
       <c r="J5" s="266">
-        <v>102.684</v>
+        <v>96.951999999999998</v>
       </c>
       <c r="K5" s="99">
         <v>21</v>
       </c>
       <c r="L5" s="40">
-        <v>15123</v>
+        <v>14125</v>
       </c>
       <c r="M5" s="40">
         <f>L5*0.5</f>
-        <v>7561.5</v>
+        <v>7062.5</v>
       </c>
       <c r="N5" s="269">
-        <v>85.6</v>
+        <v>84.2</v>
       </c>
       <c r="O5" s="40">
-        <v>0.63400000000000001</v>
+        <v>0.67600000000000005</v>
       </c>
       <c r="P5" s="270">
         <v>1</v>
@@ -22001,50 +22004,50 @@
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D6" s="82">
         <f>F6/F4</f>
-        <v>0.74184585080773002</v>
+        <v>0.70595795072435885</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="263">
         <f>J6-H6-I6</f>
-        <v>615.39599999999996</v>
+        <v>594.35799999999995</v>
       </c>
       <c r="G6" s="40">
         <v>0</v>
       </c>
       <c r="H6" s="40">
-        <v>-66.024000000000001</v>
+        <v>-64.116</v>
       </c>
       <c r="I6" s="40">
-        <v>-11.209</v>
+        <v>-11.206</v>
       </c>
       <c r="J6" s="266">
-        <v>538.16300000000001</v>
+        <v>519.03599999999994</v>
       </c>
       <c r="K6" s="99">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L6" s="40">
-        <v>82125</v>
+        <v>79125</v>
       </c>
       <c r="M6" s="40">
-        <f>L6*(1-Q6)*0.9</f>
-        <v>54592.795127040154</v>
+        <f>L6*(1-Q6)</f>
+        <v>60565.388410688502</v>
       </c>
       <c r="N6" s="269">
-        <v>77.8</v>
+        <v>76.38</v>
       </c>
       <c r="O6" s="40">
-        <v>3.93</v>
+        <v>3.35</v>
       </c>
       <c r="P6" s="270">
         <f>100%-C35</f>
-        <v>0.97447613455402915</v>
+        <v>0.97379757858799776</v>
       </c>
       <c r="Q6" s="271">
         <f>C18</f>
-        <v>0.26138616435595946</v>
+        <v>0.23456065199761764</v>
       </c>
       <c r="R6" s="38"/>
       <c r="S6" s="94"/>
@@ -22073,35 +22076,35 @@
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D7" s="82">
         <f>F7/F4</f>
-        <v>3.6246288637051309E-2</v>
+        <v>1.6419670822658293E-2</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>204</v>
       </c>
       <c r="F7" s="263">
         <f>J7</f>
-        <v>30.068000000000001</v>
+        <v>13.824</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
       <c r="I7" s="40"/>
       <c r="J7" s="266">
-        <v>30.068000000000001</v>
+        <v>13.824</v>
       </c>
       <c r="K7" s="99">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L7" s="40">
-        <v>11201</v>
-      </c>
-      <c r="M7" s="40">
-        <v>1295</v>
+        <v>5125</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="N7" s="269">
-        <v>72.510000000000005</v>
+        <v>50.5</v>
       </c>
       <c r="O7" s="40">
-        <v>0.14799999999999999</v>
+        <v>0.19</v>
       </c>
       <c r="P7" s="270"/>
       <c r="Q7" s="271"/>
@@ -22122,14 +22125,14 @@
     <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D8" s="82">
         <f>F8/F4</f>
-        <v>8.6188003814129888E-2</v>
+        <v>9.3025797079759651E-2</v>
       </c>
       <c r="E8" s="224" t="s">
         <v>189</v>
       </c>
       <c r="F8" s="263">
         <f>J8</f>
-        <v>71.497</v>
+        <v>78.319999999999993</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>66</v>
@@ -22141,7 +22144,7 @@
         <v>66</v>
       </c>
       <c r="J8" s="266">
-        <v>71.497</v>
+        <v>78.319999999999993</v>
       </c>
       <c r="K8" s="40" t="s">
         <v>66</v>
@@ -22154,7 +22157,7 @@
         <v>66</v>
       </c>
       <c r="O8" s="40">
-        <v>0.223</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="P8" s="24" t="s">
         <v>66</v>
@@ -22189,14 +22192,14 @@
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D9" s="82">
         <f>F9/F4</f>
-        <v>-5.8586192222984364E-3</v>
+        <v>4.0667904318359177E-2</v>
       </c>
       <c r="E9" s="224" t="s">
         <v>190</v>
       </c>
       <c r="F9" s="263">
         <f>J9</f>
-        <v>-4.8600000000000003</v>
+        <v>34.238999999999997</v>
       </c>
       <c r="G9" s="40" t="s">
         <v>66</v>
@@ -22208,7 +22211,7 @@
         <v>66</v>
       </c>
       <c r="J9" s="266">
-        <v>-4.8600000000000003</v>
+        <v>34.238999999999997</v>
       </c>
       <c r="K9" s="40"/>
       <c r="L9" s="40"/>
@@ -22234,17 +22237,17 @@
     <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="D10" s="82">
         <f>F10/F4</f>
-        <v>1.0547925554549654E-3</v>
+        <v>7.1859815159926697E-4</v>
       </c>
       <c r="E10" s="224" t="s">
         <v>123</v>
       </c>
       <c r="F10" s="263">
         <f>J10-G10</f>
-        <v>0.875</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="G10" s="40">
-        <v>-4.8000000000000001E-2</v>
+        <v>-7.1999999999999995E-2</v>
       </c>
       <c r="H10" s="40" t="s">
         <v>66</v>
@@ -22253,13 +22256,13 @@
         <v>0</v>
       </c>
       <c r="J10" s="266">
-        <v>0.82699999999999996</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="K10" s="99">
         <v>6</v>
       </c>
       <c r="L10" s="40">
-        <v>-28210</v>
+        <v>-36459</v>
       </c>
       <c r="M10" s="40" t="s">
         <v>66</v>
@@ -22373,7 +22376,7 @@
         <v>155</v>
       </c>
       <c r="C13" s="4">
-        <v>135.42500000000001</v>
+        <v>134.262</v>
       </c>
       <c r="E13" s="273"/>
       <c r="F13" s="16"/>
@@ -22418,7 +22421,7 @@
         <v>186</v>
       </c>
       <c r="C14" s="4">
-        <v>25.431000000000001</v>
+        <v>5.1509999999999998</v>
       </c>
       <c r="E14" s="275"/>
       <c r="F14" s="192"/>
@@ -22448,7 +22451,7 @@
     <row r="15" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <f>C13+C14</f>
-        <v>160.85600000000002</v>
+        <v>139.41300000000001</v>
       </c>
       <c r="E15" s="192"/>
       <c r="F15" s="208"/>
@@ -22497,7 +22500,7 @@
       <c r="R16" s="192"/>
       <c r="S16" s="279">
         <f>O4/J4</f>
-        <v>6.6835595270179678E-3</v>
+        <v>6.0317349213357321E-3</v>
       </c>
       <c r="U16" s="56"/>
       <c r="V16" s="205"/>
@@ -22520,7 +22523,7 @@
       <c r="H17" s="276"/>
       <c r="I17" s="276">
         <f>J4-I4-H4</f>
-        <v>829.4989999999998</v>
+        <v>841.84499999999991</v>
       </c>
       <c r="J17" s="276"/>
       <c r="K17" s="277"/>
@@ -22545,11 +22548,11 @@
     <row r="18" spans="2:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="82">
         <f>C15/F4</f>
-        <v>0.1939082414860159</v>
+        <v>0.16558995720480763</v>
       </c>
       <c r="C18" s="82">
         <f>C15/F6</f>
-        <v>0.26138616435595946</v>
+        <v>0.23456065199761764</v>
       </c>
       <c r="E18" s="192"/>
       <c r="F18" s="208"/>
@@ -22667,7 +22670,7 @@
       </c>
       <c r="C21" s="294">
         <f>J8</f>
-        <v>71.497</v>
+        <v>78.319999999999993</v>
       </c>
       <c r="E21" s="209"/>
       <c r="F21" s="208"/>
@@ -22710,7 +22713,7 @@
       </c>
       <c r="C22" s="294">
         <f>J9</f>
-        <v>-4.8600000000000003</v>
+        <v>34.238999999999997</v>
       </c>
       <c r="E22" s="192"/>
       <c r="F22" s="208"/>
@@ -22753,7 +22756,7 @@
       <c r="B23" s="44"/>
       <c r="C23" s="4">
         <f>SUM(C21:C22)</f>
-        <v>66.637</v>
+        <v>112.559</v>
       </c>
       <c r="E23" s="192"/>
       <c r="F23" s="208"/>
@@ -23157,11 +23160,11 @@
     </row>
     <row r="34" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B34" s="255">
-        <v>13.736000000000001</v>
+        <v>13.6</v>
       </c>
       <c r="C34" s="82">
         <f>B34/J4</f>
-        <v>1.8602912596376659E-2</v>
+        <v>1.8306537587629089E-2</v>
       </c>
       <c r="D34" s="251" t="s">
         <v>184</v>
@@ -23198,7 +23201,7 @@
     <row r="35" spans="2:47" x14ac:dyDescent="0.25">
       <c r="C35" s="82">
         <f>B34/J6</f>
-        <v>2.5523865445970829E-2</v>
+        <v>2.6202421412002252E-2</v>
       </c>
       <c r="D35" s="251" t="s">
         <v>34</v>
@@ -23214,7 +23217,7 @@
       <c r="AL35" s="297"/>
       <c r="AM35" s="298"/>
       <c r="AP35" s="36">
-        <v>1.54E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AQ35" s="42"/>
       <c r="AR35" s="42"/>
@@ -23239,7 +23242,7 @@
       </c>
       <c r="AI36" s="37"/>
       <c r="AJ36" s="297">
-        <v>6.7999999999999996E-3</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="AK36" s="297"/>
       <c r="AL36" s="297"/>
@@ -23303,13 +23306,13 @@
       </c>
       <c r="AI38" s="37"/>
       <c r="AJ38" s="297">
-        <v>6.1000000000000004E-3</v>
+        <v>6.4000000000000003E-3</v>
       </c>
       <c r="AK38" s="297"/>
       <c r="AL38" s="297"/>
       <c r="AM38" s="298"/>
       <c r="AP38" s="36">
-        <v>4.8999999999999998E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="AQ38" s="42"/>
       <c r="AR38" s="42"/>
@@ -23397,7 +23400,7 @@
       </c>
       <c r="AI40" s="37"/>
       <c r="AJ40" s="297">
-        <v>7.1999999999999998E-3</v>
+        <v>-3.2000000000000002E-3</v>
       </c>
       <c r="AK40" s="297"/>
       <c r="AL40" s="297"/>
@@ -23445,7 +23448,7 @@
       <c r="AL41" s="43"/>
       <c r="AM41" s="43"/>
       <c r="AP41" s="36">
-        <v>-6.9999999999999999E-4</v>
+        <v>-5.9999999999999995E-4</v>
       </c>
       <c r="AQ41" s="42"/>
       <c r="AR41" s="42"/>
@@ -23503,13 +23506,13 @@
       <c r="T43" s="44"/>
       <c r="AJ43" s="297">
         <f>SUM(AJ36:AM40)</f>
-        <v>2.01E-2</v>
+        <v>9.300000000000001E-3</v>
       </c>
       <c r="AK43" s="297"/>
       <c r="AL43" s="297"/>
       <c r="AM43" s="298"/>
       <c r="AP43" s="36">
-        <v>2.0000000000000001E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="AQ43" s="42"/>
       <c r="AR43" s="42"/>
@@ -23569,7 +23572,7 @@
         <v>153</v>
       </c>
       <c r="AJ45" s="297">
-        <v>1.49E-2</v>
+        <v>6.3E-3</v>
       </c>
       <c r="AK45" s="297"/>
       <c r="AL45" s="297"/>
@@ -23712,7 +23715,7 @@
       </c>
       <c r="AP49" s="36">
         <f>SUM(AP35:AP46)</f>
-        <v>2.01E-2</v>
+        <v>9.2999999999999992E-3</v>
       </c>
     </row>
     <row r="50" spans="5:69" x14ac:dyDescent="0.25">
@@ -23782,7 +23785,7 @@
       <c r="Q52" s="192"/>
       <c r="R52" s="192"/>
       <c r="AP52" s="35">
-        <v>1.49E-2</v>
+        <v>6.3E-3</v>
       </c>
     </row>
     <row r="53" spans="5:69" x14ac:dyDescent="0.25">
@@ -24007,7 +24010,7 @@
         <v>178435</v>
       </c>
       <c r="AP58" s="82">
-        <f t="shared" ref="AP58:AP59" si="0">AO58/$AO$61</f>
+        <f>AO58/$AO$61</f>
         <v>1.1907077939437342E-3</v>
       </c>
       <c r="AT58" s="187">
@@ -24017,7 +24020,7 @@
         <v>68</v>
       </c>
       <c r="BP58" s="18">
-        <v>0.13800000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="BQ58" s="21">
         <v>0.05</v>
@@ -24060,14 +24063,14 @@
         <v>133570</v>
       </c>
       <c r="AP59" s="82">
-        <f t="shared" si="0"/>
+        <f>AO59/$AO$61</f>
         <v>8.9132087335480462E-4</v>
       </c>
       <c r="BO59" s="20" t="s">
         <v>67</v>
       </c>
       <c r="BP59" s="221">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="BQ59" s="19">
         <v>4.9000000000000004</v>
@@ -24530,7 +24533,7 @@
       </c>
       <c r="AM74" s="70">
         <f>H4</f>
-        <v>-79.911000000000001</v>
+        <v>-87.734999999999999</v>
       </c>
       <c r="BU74" s="44">
         <v>711000000</v>
@@ -24571,7 +24574,7 @@
       </c>
       <c r="AM75" s="70">
         <f>J10</f>
-        <v>0.82699999999999996</v>
+        <v>0.53300000000000003</v>
       </c>
       <c r="AO75" s="304" t="s">
         <v>156</v>
@@ -24731,7 +24734,7 @@
       </c>
       <c r="AM78" s="189">
         <f>1-(J6/F6)</f>
-        <v>0.12550130322589026</v>
+        <v>0.12672833544765949</v>
       </c>
       <c r="AO78" s="68" t="s">
         <v>35</v>
@@ -24770,7 +24773,7 @@
       </c>
       <c r="AM79" s="112">
         <f>1-(J5/F5)</f>
-        <v>0.11912911444527374</v>
+        <v>0.19589287639648012</v>
       </c>
       <c r="AO79" s="68" t="s">
         <v>204</v>
@@ -24845,7 +24848,7 @@
       </c>
       <c r="AM82" s="188">
         <f>(F4/J4)-1</f>
-        <v>0.12347046706366238</v>
+        <v>0.13327832398264117</v>
       </c>
       <c r="AO82" s="68" t="s">
         <v>101</v>
@@ -25192,18 +25195,18 @@
       </c>
       <c r="AN95" s="294">
         <f>'Credit Risk Tables'!J7</f>
-        <v>30.068000000000001</v>
+        <v>13.824</v>
       </c>
       <c r="AO95" s="4">
         <v>14.7</v>
       </c>
       <c r="AP95" s="294">
         <f>AN95-AO95</f>
-        <v>15.368000000000002</v>
+        <v>-0.87599999999999945</v>
       </c>
       <c r="AQ95" s="4">
         <f>AN95/AP95</f>
-        <v>1.9565330557001559</v>
+        <v>-15.780821917808229</v>
       </c>
       <c r="AZ95" s="77"/>
       <c r="BA95" s="244"/>
@@ -25880,6 +25883,111 @@
         <v>0</v>
       </c>
       <c r="AA145" s="119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W148" s="102">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="149" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W149" s="98"/>
+      <c r="X149" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y149" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z149" s="88" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA149" s="89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="150" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W150" s="23">
+        <v>1</v>
+      </c>
+      <c r="X150" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y150" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z150" s="84">
+        <v>0.4824</v>
+      </c>
+      <c r="AA150" s="118">
+        <v>0.52300000000000002</v>
+      </c>
+    </row>
+    <row r="151" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W151" s="23">
+        <v>2</v>
+      </c>
+      <c r="X151" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y151" s="97" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z151" s="84">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="AA151" s="118">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="152" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W152" s="23">
+        <v>3</v>
+      </c>
+      <c r="X152" s="96" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y152" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z152" s="121">
+        <v>0.32</v>
+      </c>
+      <c r="AA152" s="156">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="153" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W153" s="23">
+        <v>4</v>
+      </c>
+      <c r="X153" s="97" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y153" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z153" s="84">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AA153" s="118">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="23:27" x14ac:dyDescent="0.25">
+      <c r="W154" s="22">
+        <v>5</v>
+      </c>
+      <c r="X154" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y154" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z154" s="86">
+        <v>0</v>
+      </c>
+      <c r="AA154" s="119">
         <v>0</v>
       </c>
     </row>
@@ -25957,7 +26065,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26142,8 +26250,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q315"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26170,7 +26278,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="120">
-        <v>2.7538990223589292E-2</v>
+        <v>2.7045167236918379E-2</v>
       </c>
       <c r="C2" s="215">
         <f>AVERAGE($B$2:$B$202)</f>
@@ -26186,7 +26294,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="120">
-        <v>2.6175154413272166E-2</v>
+        <v>2.3904760962183986E-2</v>
       </c>
       <c r="C3" s="215">
         <f t="shared" ref="C3:C66" si="0">AVERAGE($B$2:$B$203)</f>
@@ -26202,7 +26310,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="120">
-        <v>2.3464186653468201E-2</v>
+        <v>2.1603660596083377E-2</v>
       </c>
       <c r="C4" s="215">
         <f t="shared" si="0"/>
@@ -26218,7 +26326,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="120">
-        <v>2.0811674921631201E-2</v>
+        <v>1.9924891708791987E-2</v>
       </c>
       <c r="C5" s="215">
         <f t="shared" si="0"/>
@@ -26234,7 +26342,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="120">
-        <v>1.9578768201385599E-2</v>
+        <v>1.8795128400195395E-2</v>
       </c>
       <c r="C6" s="215">
         <f t="shared" si="0"/>
@@ -26253,7 +26361,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="120">
-        <v>1.8773493030693669E-2</v>
+        <v>1.8136468756324804E-2</v>
       </c>
       <c r="C7" s="215">
         <f t="shared" si="0"/>
@@ -26269,7 +26377,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="120">
-        <v>1.7809812530165472E-2</v>
+        <v>1.7927162195716238E-2</v>
       </c>
       <c r="C8" s="215">
         <f t="shared" si="0"/>
@@ -26285,7 +26393,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="120">
-        <v>1.7383613835201994E-2</v>
+        <v>1.7747018684793562E-2</v>
       </c>
       <c r="C9" s="215">
         <f t="shared" si="0"/>
@@ -26301,7 +26409,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="120">
-        <v>1.7184630522191321E-2</v>
+        <v>1.7329283087763811E-2</v>
       </c>
       <c r="C10" s="215">
         <f t="shared" si="0"/>
@@ -26317,7 +26425,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="120">
-        <v>1.5794804338968228E-2</v>
+        <v>1.6245822084007003E-2</v>
       </c>
       <c r="C11" s="215">
         <f t="shared" si="0"/>
@@ -26333,7 +26441,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="120">
-        <v>1.4686433846166231E-2</v>
+        <v>1.6215952440089339E-2</v>
       </c>
       <c r="C12" s="215">
         <f t="shared" si="0"/>
@@ -26349,7 +26457,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="120">
-        <v>1.449786664032068E-2</v>
+        <v>1.4966974253448648E-2</v>
       </c>
       <c r="C13" s="215">
         <f t="shared" si="0"/>
@@ -26365,7 +26473,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="120">
-        <v>1.4409305989080376E-2</v>
+        <v>1.4755062591656685E-2</v>
       </c>
       <c r="C14" s="215">
         <f t="shared" si="0"/>
@@ -26381,7 +26489,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="120">
-        <v>1.4404284098204045E-2</v>
+        <v>1.4601423232270183E-2</v>
       </c>
       <c r="C15" s="215">
         <f t="shared" si="0"/>
@@ -26397,7 +26505,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="120">
-        <v>1.3648127397534097E-2</v>
+        <v>1.4407109514828931E-2</v>
       </c>
       <c r="C16" s="215">
         <f t="shared" si="0"/>
@@ -26413,7 +26521,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="120">
-        <v>1.3559905308638615E-2</v>
+        <v>1.400765392540677E-2</v>
       </c>
       <c r="C17" s="215">
         <f t="shared" si="0"/>
@@ -26429,7 +26537,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="120">
-        <v>1.3551353397569917E-2</v>
+        <v>1.3808527746987919E-2</v>
       </c>
       <c r="C18" s="215">
         <f t="shared" si="0"/>
@@ -26445,7 +26553,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="120">
-        <v>1.3545218864184213E-2</v>
+        <v>1.3785320492214644E-2</v>
       </c>
       <c r="C19" s="215">
         <f t="shared" si="0"/>
@@ -26461,7 +26569,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="120">
-        <v>1.3260831776829964E-2</v>
+        <v>1.3782696492379233E-2</v>
       </c>
       <c r="C20" s="215">
         <f t="shared" si="0"/>
@@ -26477,7 +26585,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="120">
-        <v>1.3045521512526304E-2</v>
+        <v>1.3316895963347531E-2</v>
       </c>
       <c r="C21" s="215">
         <f t="shared" si="0"/>
@@ -26493,7 +26601,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="120">
-        <v>1.2992104519820752E-2</v>
+        <v>1.3290563984191131E-2</v>
       </c>
       <c r="C22" s="215">
         <f t="shared" si="0"/>
@@ -26509,7 +26617,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="120">
-        <v>1.2952178621811184E-2</v>
+        <v>1.3290102202738616E-2</v>
       </c>
       <c r="C23" s="215">
         <f t="shared" si="0"/>
@@ -26525,7 +26633,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="120">
-        <v>1.2944305298576649E-2</v>
+        <v>1.3154691649279415E-2</v>
       </c>
       <c r="C24" s="215">
         <f t="shared" si="0"/>
@@ -26541,7 +26649,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="120">
-        <v>1.2746180150098659E-2</v>
+        <v>1.24889344917126E-2</v>
       </c>
       <c r="C25" s="215">
         <f t="shared" si="0"/>
@@ -26557,7 +26665,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="120">
-        <v>1.2201966476852724E-2</v>
+        <v>1.2457824356290255E-2</v>
       </c>
       <c r="C26" s="215">
         <f t="shared" si="0"/>
@@ -26573,7 +26681,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="120">
-        <v>1.2127343849557545E-2</v>
+        <v>1.2452337038115928E-2</v>
       </c>
       <c r="C27" s="215">
         <f t="shared" si="0"/>
@@ -26589,7 +26697,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="120">
-        <v>1.2004386987440666E-2</v>
+        <v>1.2344434418284821E-2</v>
       </c>
       <c r="C28" s="215">
         <f t="shared" si="0"/>
@@ -26605,7 +26713,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="120">
-        <v>1.1400472902684712E-2</v>
+        <v>1.1674234227663366E-2</v>
       </c>
       <c r="C29" s="215">
         <f t="shared" si="0"/>
@@ -26621,7 +26729,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="120">
-        <v>1.1101553557256413E-2</v>
+        <v>1.1313987087633696E-2</v>
       </c>
       <c r="C30" s="215">
         <f t="shared" si="0"/>
@@ -26637,7 +26745,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="120">
-        <v>1.1071060939994787E-2</v>
+        <v>1.1295592404275722E-2</v>
       </c>
       <c r="C31" s="215">
         <f t="shared" si="0"/>
@@ -26653,7 +26761,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="120">
-        <v>1.088437447963592E-2</v>
+        <v>1.1087344540907146E-2</v>
       </c>
       <c r="C32" s="215">
         <f t="shared" si="0"/>
@@ -26669,7 +26777,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="120">
-        <v>1.0571910778369747E-2</v>
+        <v>1.0844735656461549E-2</v>
       </c>
       <c r="C33" s="215">
         <f t="shared" si="0"/>
@@ -26685,7 +26793,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="120">
-        <v>1.0486020124955267E-2</v>
+        <v>1.0837174856599104E-2</v>
       </c>
       <c r="C34" s="215">
         <f t="shared" si="0"/>
@@ -26701,7 +26809,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="120">
-        <v>1.0290284203770549E-2</v>
+        <v>1.0813252683352153E-2</v>
       </c>
       <c r="C35" s="215">
         <f t="shared" si="0"/>
@@ -26717,7 +26825,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="120">
-        <v>1.0147863308924242E-2</v>
+        <v>1.0436510926848695E-2</v>
       </c>
       <c r="C36" s="215">
         <f t="shared" si="0"/>
@@ -26733,7 +26841,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="120">
-        <v>1.0017902508887424E-2</v>
+        <v>1.0355471201628901E-2</v>
       </c>
       <c r="C37" s="215">
         <f t="shared" si="0"/>
@@ -26749,7 +26857,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="120">
-        <v>9.6768736269436818E-3</v>
+        <v>1.0336396539525701E-2</v>
       </c>
       <c r="C38" s="215">
         <f t="shared" si="0"/>
@@ -26765,7 +26873,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="120">
-        <v>9.6377781494518429E-3</v>
+        <v>9.9635364336205165E-3</v>
       </c>
       <c r="C39" s="215">
         <f t="shared" si="0"/>
@@ -26781,7 +26889,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="120">
-        <v>9.3896733693005566E-3</v>
+        <v>9.6009794199983598E-3</v>
       </c>
       <c r="C40" s="215">
         <f t="shared" si="0"/>
@@ -26797,7 +26905,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="120">
-        <v>9.3418450702200135E-3</v>
+        <v>9.5581465570284962E-3</v>
       </c>
       <c r="C41" s="215">
         <f t="shared" si="0"/>
@@ -26813,7 +26921,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="120">
-        <v>9.0548278345516531E-3</v>
+        <v>9.5418652509790397E-3</v>
       </c>
       <c r="C42" s="215">
         <f t="shared" si="0"/>
@@ -26829,7 +26937,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="120">
-        <v>8.8717789268286575E-3</v>
+        <v>9.0132674831253663E-3</v>
       </c>
       <c r="C43" s="215">
         <f t="shared" si="0"/>
@@ -26845,7 +26953,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="120">
-        <v>8.6618696394714645E-3</v>
+        <v>8.9809918986178735E-3</v>
       </c>
       <c r="C44" s="215">
         <f t="shared" si="0"/>
@@ -26861,7 +26969,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="120">
-        <v>8.6058060203857388E-3</v>
+        <v>8.9695553703790041E-3</v>
       </c>
       <c r="C45" s="215">
         <f t="shared" si="0"/>
@@ -26877,7 +26985,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="120">
-        <v>8.5170073349799397E-3</v>
+        <v>8.8735299252237741E-3</v>
       </c>
       <c r="C46" s="215">
         <f t="shared" si="0"/>
@@ -26893,7 +27001,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="120">
-        <v>8.4545708958043697E-3</v>
+        <v>8.830250797298737E-3</v>
       </c>
       <c r="C47" s="215">
         <f t="shared" si="0"/>
@@ -26909,7 +27017,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="120">
-        <v>8.2135133901149286E-3</v>
+        <v>8.8113767176745388E-3</v>
       </c>
       <c r="C48" s="215">
         <f t="shared" si="0"/>
@@ -26925,7 +27033,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="120">
-        <v>8.0682192187579681E-3</v>
+        <v>8.5541157455958083E-3</v>
       </c>
       <c r="C49" s="215">
         <f t="shared" si="0"/>
@@ -26941,7 +27049,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="120">
-        <v>7.9825308419737961E-3</v>
+        <v>8.3886403495779891E-3</v>
       </c>
       <c r="C50" s="215">
         <f t="shared" si="0"/>
@@ -26957,7 +27065,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="120">
-        <v>7.9637372411657734E-3</v>
+        <v>8.3736105788035642E-3</v>
       </c>
       <c r="C51" s="215">
         <f t="shared" si="0"/>
@@ -26973,7 +27081,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="120">
-        <v>7.9136900695474868E-3</v>
+        <v>8.1142680768890689E-3</v>
       </c>
       <c r="C52" s="215">
         <f t="shared" si="0"/>
@@ -26989,7 +27097,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="120">
-        <v>7.883877425358574E-3</v>
+        <v>8.1068374830790598E-3</v>
       </c>
       <c r="C53" s="215">
         <f t="shared" si="0"/>
@@ -27005,7 +27113,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="120">
-        <v>7.7163517793967353E-3</v>
+        <v>8.0098082282224828E-3</v>
       </c>
       <c r="C54" s="215">
         <f t="shared" si="0"/>
@@ -27021,7 +27129,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="120">
-        <v>7.6751519147574545E-3</v>
+        <v>7.8078792513262404E-3</v>
       </c>
       <c r="C55" s="215">
         <f t="shared" si="0"/>
@@ -27037,7 +27145,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="120">
-        <v>7.5514212571688158E-3</v>
+        <v>7.7291554461632016E-3</v>
       </c>
       <c r="C56" s="215">
         <f t="shared" si="0"/>
@@ -27053,7 +27161,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="120">
-        <v>7.4724118813838964E-3</v>
+        <v>7.6446839245256715E-3</v>
       </c>
       <c r="C57" s="215">
         <f t="shared" si="0"/>
@@ -27069,7 +27177,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="120">
-        <v>7.4122524951454353E-3</v>
+        <v>7.5549132567558856E-3</v>
       </c>
       <c r="C58" s="215">
         <f t="shared" si="0"/>
@@ -27085,7 +27193,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="120">
-        <v>7.3294935411766828E-3</v>
+        <v>7.4397410750912021E-3</v>
       </c>
       <c r="C59" s="215">
         <f t="shared" si="0"/>
@@ -27101,7 +27209,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="120">
-        <v>7.2687594965938187E-3</v>
+        <v>7.439224005763365E-3</v>
       </c>
       <c r="C60" s="215">
         <f t="shared" si="0"/>
@@ -27117,7 +27225,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="120">
-        <v>6.8481960801705143E-3</v>
+        <v>7.4173665206023953E-3</v>
       </c>
       <c r="C61" s="215">
         <f t="shared" si="0"/>
@@ -27133,7 +27241,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="120">
-        <v>6.8370576896229114E-3</v>
+        <v>7.302752836209076E-3</v>
       </c>
       <c r="C62" s="215">
         <f t="shared" si="0"/>
@@ -27149,7 +27257,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="120">
-        <v>6.731083246290904E-3</v>
+        <v>7.2060601540586602E-3</v>
       </c>
       <c r="C63" s="215">
         <f t="shared" si="0"/>
@@ -27165,7 +27273,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="120">
-        <v>6.6698221792003123E-3</v>
+        <v>7.0279479790355051E-3</v>
       </c>
       <c r="C64" s="215">
         <f t="shared" si="0"/>
@@ -27181,7 +27289,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="120">
-        <v>6.6071639813753379E-3</v>
+        <v>6.9409638201818448E-3</v>
       </c>
       <c r="C65" s="215">
         <f t="shared" si="0"/>
@@ -27197,7 +27305,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="120">
-        <v>6.5822842029454173E-3</v>
+        <v>6.8403963069613482E-3</v>
       </c>
       <c r="C66" s="215">
         <f t="shared" si="0"/>
@@ -27213,7 +27321,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="120">
-        <v>6.5208647937831932E-3</v>
+        <v>6.7237767149497417E-3</v>
       </c>
       <c r="C67" s="215">
         <f t="shared" ref="C67:C131" si="1">AVERAGE($B$2:$B$203)</f>
@@ -27229,7 +27337,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="120">
-        <v>6.4987666602881302E-3</v>
+        <v>6.6724867121063141E-3</v>
       </c>
       <c r="C68" s="215">
         <f t="shared" si="1"/>
@@ -27245,7 +27353,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="120">
-        <v>6.3058261481941727E-3</v>
+        <v>6.6718843296525157E-3</v>
       </c>
       <c r="C69" s="215">
         <f t="shared" si="1"/>
@@ -27261,7 +27369,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="120">
-        <v>6.1963349339672572E-3</v>
+        <v>6.603022666631814E-3</v>
       </c>
       <c r="C70" s="215">
         <f t="shared" si="1"/>
@@ -27277,7 +27385,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="120">
-        <v>6.0920297455003443E-3</v>
+        <v>6.3044161513552488E-3</v>
       </c>
       <c r="C71" s="215">
         <f t="shared" si="1"/>
@@ -27293,7 +27401,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="120">
-        <v>6.0099686825839521E-3</v>
+        <v>6.23035426677521E-3</v>
       </c>
       <c r="C72" s="215">
         <f t="shared" si="1"/>
@@ -27309,7 +27417,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="120">
-        <v>5.8800514446850586E-3</v>
+        <v>6.1379660873850973E-3</v>
       </c>
       <c r="C73" s="215">
         <f t="shared" si="1"/>
@@ -27325,7 +27433,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="120">
-        <v>5.8381302673505674E-3</v>
+        <v>5.4219477370113338E-3</v>
       </c>
       <c r="C74" s="215">
         <f t="shared" si="1"/>
@@ -27340,7 +27448,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="120">
-        <v>5.7261858380325964E-3</v>
+        <v>5.356228620258161E-3</v>
       </c>
       <c r="C75" s="215">
         <f t="shared" si="1"/>
@@ -27355,7 +27463,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="120">
-        <v>5.2766908387614966E-3</v>
+        <v>5.3309906093833093E-3</v>
       </c>
       <c r="C76" s="215">
         <f t="shared" si="1"/>
@@ -27370,7 +27478,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="120">
-        <v>5.2595503270582442E-3</v>
+        <v>5.304312546073533E-3</v>
       </c>
       <c r="C77" s="215">
         <f t="shared" si="1"/>
@@ -27385,7 +27493,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="120">
-        <v>5.2365108958190741E-3</v>
+        <v>5.2854903721699835E-3</v>
       </c>
       <c r="C78" s="215">
         <f t="shared" si="1"/>
@@ -27400,7 +27508,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="120">
-        <v>5.2364779439928412E-3</v>
+        <v>5.165855444320579E-3</v>
       </c>
       <c r="C79" s="215">
         <f t="shared" si="1"/>
@@ -27415,7 +27523,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="120">
-        <v>5.1467129096084219E-3</v>
+        <v>5.0715470293606771E-3</v>
       </c>
       <c r="C80" s="215">
         <f t="shared" si="1"/>
@@ -27430,7 +27538,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="120">
-        <v>5.0749588942454312E-3</v>
+        <v>4.9086085806584745E-3</v>
       </c>
       <c r="C81" s="215">
         <f t="shared" si="1"/>
@@ -27445,7 +27553,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="120">
-        <v>4.8906189761698743E-3</v>
+        <v>4.8661613109304176E-3</v>
       </c>
       <c r="C82" s="215">
         <f t="shared" si="1"/>
@@ -27460,7 +27568,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="120">
-        <v>4.8822368329879337E-3</v>
+        <v>4.7596380442114427E-3</v>
       </c>
       <c r="C83" s="215">
         <f t="shared" si="1"/>
@@ -27475,7 +27583,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="120">
-        <v>4.7936650182820858E-3</v>
+        <v>4.6736227001118276E-3</v>
       </c>
       <c r="C84" s="215">
         <f t="shared" si="1"/>
@@ -27490,7 +27598,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="120">
-        <v>4.7287124143296968E-3</v>
+        <v>4.6391174750034488E-3</v>
       </c>
       <c r="C85" s="215">
         <f t="shared" si="1"/>
@@ -27505,7 +27613,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="120">
-        <v>4.6244217380966707E-3</v>
+        <v>4.5528456807515695E-3</v>
       </c>
       <c r="C86" s="215">
         <f t="shared" si="1"/>
@@ -27520,7 +27628,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="120">
-        <v>4.4780158971009891E-3</v>
+        <v>4.349327477692384E-3</v>
       </c>
       <c r="C87" s="215">
         <f t="shared" si="1"/>
@@ -27535,7 +27643,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="120">
-        <v>4.3730006228254832E-3</v>
+        <v>4.1292133729805783E-3</v>
       </c>
       <c r="C88" s="215">
         <f t="shared" si="1"/>
@@ -27550,7 +27658,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="120">
-        <v>4.2492448862754516E-3</v>
+        <v>4.0444672894074099E-3</v>
       </c>
       <c r="C89" s="215">
         <f t="shared" si="1"/>
@@ -27565,7 +27673,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="120">
-        <v>4.2258105687921496E-3</v>
+        <v>3.9105062446114971E-3</v>
       </c>
       <c r="C90" s="215">
         <f t="shared" si="1"/>
@@ -27580,7 +27688,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="120">
-        <v>4.0224209274573562E-3</v>
+        <v>3.9062833691188023E-3</v>
       </c>
       <c r="C91" s="215">
         <f t="shared" si="1"/>
@@ -27595,7 +27703,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="120">
-        <v>3.9982923929708222E-3</v>
+        <v>3.8940015783066888E-3</v>
       </c>
       <c r="C92" s="215">
         <f t="shared" si="1"/>
@@ -27610,7 +27718,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="120">
-        <v>3.9638300281556373E-3</v>
+        <v>3.8812537817998999E-3</v>
       </c>
       <c r="C93" s="215">
         <f t="shared" si="1"/>
@@ -27625,7 +27733,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="120">
-        <v>3.9200268048395666E-3</v>
+        <v>3.7128962654241413E-3</v>
       </c>
       <c r="C94" s="215">
         <f t="shared" si="1"/>
@@ -27640,7 +27748,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="120">
-        <v>3.8416751225075038E-3</v>
+        <v>3.4870783846391302E-3</v>
       </c>
       <c r="C95" s="215">
         <f t="shared" si="1"/>
@@ -27655,7 +27763,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="120">
-        <v>3.8084889614445755E-3</v>
+        <v>3.3992419228086267E-3</v>
       </c>
       <c r="C96" s="215">
         <f t="shared" si="1"/>
@@ -27670,7 +27778,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="120">
-        <v>3.8074484716491843E-3</v>
+        <v>3.361303313740524E-3</v>
       </c>
       <c r="C97" s="215">
         <f t="shared" si="1"/>
@@ -27685,7 +27793,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="120">
-        <v>3.7633254550290323E-3</v>
+        <v>3.3140140961680315E-3</v>
       </c>
       <c r="C98" s="215">
         <f t="shared" si="1"/>
@@ -27700,7 +27808,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="120">
-        <v>3.6072805072487231E-3</v>
+        <v>3.182964230650794E-3</v>
       </c>
       <c r="C99" s="215">
         <f t="shared" si="1"/>
@@ -27715,7 +27823,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="120">
-        <v>3.3347110225668336E-3</v>
+        <v>3.1654316792252757E-3</v>
       </c>
       <c r="C100" s="215">
         <f t="shared" si="1"/>
@@ -27730,7 +27838,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="120">
-        <v>3.3214781128092911E-3</v>
+        <v>3.1492288253594479E-3</v>
       </c>
       <c r="C101" s="215">
         <f t="shared" si="1"/>
@@ -27745,7 +27853,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="120">
-        <v>3.2176313684901714E-3</v>
+        <v>3.1384277556665775E-3</v>
       </c>
       <c r="C102" s="215">
         <f t="shared" si="1"/>
@@ -27760,7 +27868,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="120">
-        <v>3.1626201442374788E-3</v>
+        <v>2.7676953701666518E-3</v>
       </c>
       <c r="C103" s="215">
         <f t="shared" si="1"/>
@@ -27775,7 +27883,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="120">
-        <v>3.0944504455674097E-3</v>
+        <v>2.757823827014803E-3</v>
       </c>
       <c r="C104" s="215">
         <f t="shared" si="1"/>
@@ -27790,7 +27898,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="120">
-        <v>3.0823578746581671E-3</v>
+        <v>2.7097665566285342E-3</v>
       </c>
       <c r="C105" s="215">
         <f t="shared" si="1"/>
@@ -27805,7 +27913,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="120">
-        <v>2.8134838196032202E-3</v>
+        <v>2.6941034532339016E-3</v>
       </c>
       <c r="C106" s="215">
         <f t="shared" si="1"/>
@@ -27820,7 +27928,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="120">
-        <v>2.713956163343037E-3</v>
+        <v>2.5378013717921978E-3</v>
       </c>
       <c r="C107" s="215">
         <f t="shared" si="1"/>
@@ -27835,7 +27943,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="120">
-        <v>2.6796669280809674E-3</v>
+        <v>2.4922277625296025E-3</v>
       </c>
       <c r="C108" s="215">
         <f t="shared" si="1"/>
@@ -27850,7 +27958,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="120">
-        <v>2.6510986745924962E-3</v>
+        <v>2.277405956812435E-3</v>
       </c>
       <c r="C109" s="215">
         <f t="shared" si="1"/>
@@ -27865,7 +27973,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="120">
-        <v>2.6461835949039068E-3</v>
+        <v>2.174031821209062E-3</v>
       </c>
       <c r="C110" s="215">
         <f t="shared" si="1"/>
@@ -27880,7 +27988,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="120">
-        <v>2.5477842639907771E-3</v>
+        <v>2.1326922140377895E-3</v>
       </c>
       <c r="C111" s="215">
         <f t="shared" si="1"/>
@@ -27895,7 +28003,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="120">
-        <v>2.4011727169126291E-3</v>
+        <v>2.0481472237179996E-3</v>
       </c>
       <c r="C112" s="215">
         <f t="shared" si="1"/>
@@ -27910,7 +28018,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="120">
-        <v>2.2970995308723443E-3</v>
+        <v>1.9358285452413314E-3</v>
       </c>
       <c r="C113" s="215">
         <f t="shared" si="1"/>
@@ -27925,7 +28033,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="120">
-        <v>2.1804501521514677E-3</v>
+        <v>1.8483333359146758E-3</v>
       </c>
       <c r="C114" s="215">
         <f t="shared" si="1"/>
@@ -27940,7 +28048,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="120">
-        <v>2.1525158010601043E-3</v>
+        <v>1.781638833364099E-3</v>
       </c>
       <c r="C115" s="215">
         <f t="shared" si="1"/>
@@ -27955,7 +28063,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="120">
-        <v>2.0749072330865175E-3</v>
+        <v>1.6988457025303829E-3</v>
       </c>
       <c r="C116" s="215">
         <f t="shared" si="1"/>
@@ -27970,7 +28078,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="120">
-        <v>2.0697183143433217E-3</v>
+        <v>1.683440070836772E-3</v>
       </c>
       <c r="C117" s="215">
         <f t="shared" si="1"/>
@@ -27985,7 +28093,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="120">
-        <v>1.9060237075932489E-3</v>
+        <v>1.6212380774320108E-3</v>
       </c>
       <c r="C118" s="215">
         <f t="shared" si="1"/>
@@ -28000,7 +28108,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="120">
-        <v>1.8005989181893109E-3</v>
+        <v>1.5699138527052079E-3</v>
       </c>
       <c r="C119" s="215">
         <f t="shared" si="1"/>
@@ -28015,7 +28123,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="120">
-        <v>1.7795385160118196E-3</v>
+        <v>1.4205367674621286E-3</v>
       </c>
       <c r="C120" s="215">
         <f t="shared" si="1"/>
@@ -28030,7 +28138,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="120">
-        <v>1.6451045493905145E-3</v>
+        <v>1.3766998463060867E-3</v>
       </c>
       <c r="C121" s="215">
         <f t="shared" si="1"/>
@@ -28045,7 +28153,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="120">
-        <v>1.6021119865575009E-3</v>
+        <v>1.229614785161664E-3</v>
       </c>
       <c r="C122" s="215">
         <f t="shared" si="1"/>
@@ -28060,7 +28168,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="120">
-        <v>1.3665707949721002E-3</v>
+        <v>1.2096244012303806E-3</v>
       </c>
       <c r="C123" s="215">
         <f t="shared" si="1"/>
@@ -28075,7 +28183,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="120">
-        <v>1.2334755881539413E-3</v>
+        <v>1.1809214350173135E-3</v>
       </c>
       <c r="C124" s="215">
         <f t="shared" si="1"/>
@@ -28090,7 +28198,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="120">
-        <v>1.2161443569352075E-3</v>
+        <v>1.1655820659458092E-3</v>
       </c>
       <c r="C125" s="215">
         <f t="shared" si="1"/>
@@ -28105,7 +28213,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="253">
-        <v>1.1845293656542976E-3</v>
+        <v>1.1232624345935847E-3</v>
       </c>
       <c r="C126" s="215">
         <f t="shared" si="1"/>
@@ -28120,7 +28228,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="253">
-        <v>1.1834435138390112E-3</v>
+        <v>1.0399113448723081E-3</v>
       </c>
       <c r="C127" s="215">
         <f t="shared" si="1"/>
@@ -28135,7 +28243,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="253">
-        <v>1.1508091723830057E-3</v>
+        <v>1.0097024777435978E-3</v>
       </c>
       <c r="C128" s="215">
         <f t="shared" si="1"/>
@@ -28150,7 +28258,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="253">
-        <v>1.0159195761445207E-3</v>
+        <v>9.0792819793212903E-4</v>
       </c>
       <c r="C129" s="215">
         <f t="shared" si="1"/>
@@ -28165,7 +28273,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="253">
-        <v>9.8710701607583932E-4</v>
+        <v>9.0571893308754074E-4</v>
       </c>
       <c r="C130" s="215">
         <f t="shared" si="1"/>
@@ -28180,7 +28288,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>9.7776974515775719E-4</v>
+        <v>6.9754948048845664E-4</v>
       </c>
       <c r="C131" s="215">
         <f t="shared" si="1"/>
@@ -28195,7 +28303,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>8.7743970954118171E-4</v>
+        <v>6.2843659930169411E-4</v>
       </c>
       <c r="C132" s="215">
         <f t="shared" ref="C132:C195" si="2">AVERAGE($B$2:$B$203)</f>
@@ -28210,7 +28318,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>6.8705800341977645E-4</v>
+        <v>6.1893963323072696E-4</v>
       </c>
       <c r="C133" s="215">
         <f t="shared" si="2"/>
@@ -28225,7 +28333,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>6.1098114967575695E-4</v>
+        <v>5.6421619120872331E-4</v>
       </c>
       <c r="C134" s="215">
         <f t="shared" si="2"/>
@@ -28240,7 +28348,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>6.0880109383079509E-4</v>
+        <v>5.3032487548944688E-4</v>
       </c>
       <c r="C135" s="215">
         <f t="shared" si="2"/>
@@ -28255,7 +28363,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>5.8470717445661046E-4</v>
+        <v>5.0428471415985953E-4</v>
       </c>
       <c r="C136" s="215">
         <f t="shared" si="2"/>
@@ -28270,7 +28378,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>5.4172516658072584E-4</v>
+        <v>4.5711648109156289E-4</v>
       </c>
       <c r="C137" s="215">
         <f t="shared" si="2"/>
@@ -28285,7 +28393,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>5.1475863032430288E-4</v>
+        <v>4.3247129980915529E-4</v>
       </c>
       <c r="C138" s="215">
         <f t="shared" si="2"/>
@@ -28300,7 +28408,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>4.4944863583792422E-4</v>
+        <v>3.9178183939844903E-4</v>
       </c>
       <c r="C139" s="215">
         <f t="shared" si="2"/>
@@ -28315,7 +28423,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>4.4929766848566936E-4</v>
+        <v>3.6420198321594457E-4</v>
       </c>
       <c r="C140" s="215">
         <f t="shared" si="2"/>
@@ -28330,7 +28438,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>4.1196543597449579E-4</v>
+        <v>3.6417325560831888E-4</v>
       </c>
       <c r="C141" s="215">
         <f t="shared" si="2"/>
@@ -28345,7 +28453,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>4.0713183969113583E-4</v>
+        <v>3.58466373474702E-4</v>
       </c>
       <c r="C142" s="215">
         <f t="shared" si="2"/>
@@ -28360,7 +28468,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>3.9384740829201848E-4</v>
+        <v>3.1853974769628147E-4</v>
       </c>
       <c r="C143" s="215">
         <f t="shared" si="2"/>
@@ -28375,7 +28483,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>3.4211302945093345E-4</v>
+        <v>2.898317151535657E-4</v>
       </c>
       <c r="C144" s="215">
         <f t="shared" si="2"/>
@@ -28390,7 +28498,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>3.1919983680591622E-4</v>
+        <v>2.530936329461867E-4</v>
       </c>
       <c r="C145" s="215">
         <f t="shared" si="2"/>
@@ -28405,7 +28513,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>2.7370125900597514E-4</v>
+        <v>2.4822193594536778E-4</v>
       </c>
       <c r="C146" s="215">
         <f t="shared" si="2"/>
@@ -28420,7 +28528,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>2.6350839084243922E-4</v>
+        <v>2.4632715626623857E-4</v>
       </c>
       <c r="C147" s="215">
         <f t="shared" si="2"/>
@@ -28435,7 +28543,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>2.5486115427478213E-4</v>
+        <v>2.3683473194582833E-4</v>
       </c>
       <c r="C148" s="215">
         <f t="shared" si="2"/>
@@ -28450,7 +28558,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>2.5108296897734505E-4</v>
+        <v>2.3627415016280918E-4</v>
       </c>
       <c r="C149" s="215">
         <f t="shared" si="2"/>
@@ -28465,7 +28573,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>2.4256813271656685E-4</v>
+        <v>2.2131391372745638E-4</v>
       </c>
       <c r="C150" s="215">
         <f t="shared" si="2"/>
@@ -28480,7 +28588,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>2.2142519471729996E-4</v>
+        <v>1.8839599592692126E-4</v>
       </c>
       <c r="C151" s="215">
         <f t="shared" si="2"/>
@@ -28495,7 +28603,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>2.1357628362057244E-4</v>
+        <v>1.8744844043080134E-4</v>
       </c>
       <c r="C152" s="215">
         <f t="shared" si="2"/>
@@ -28510,7 +28618,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>2.0004548913559538E-4</v>
+        <v>1.7840391002169084E-4</v>
       </c>
       <c r="C153" s="215">
         <f t="shared" si="2"/>
@@ -28525,7 +28633,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>1.9897338344245028E-4</v>
+        <v>1.7208811580505601E-4</v>
       </c>
       <c r="C154" s="215">
         <f t="shared" si="2"/>
@@ -28540,7 +28648,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>1.9333374608214679E-4</v>
+        <v>1.4819373144525148E-4</v>
       </c>
       <c r="C155" s="215">
         <f t="shared" si="2"/>
@@ -28555,7 +28663,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>1.8282883540970011E-4</v>
+        <v>1.3688568366970313E-4</v>
       </c>
       <c r="C156" s="215">
         <f t="shared" si="2"/>
@@ -28570,7 +28678,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>1.4719652638100125E-4</v>
+        <v>1.3560021641026706E-4</v>
       </c>
       <c r="C157" s="215">
         <f t="shared" si="2"/>
@@ -28585,7 +28693,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>1.4025003909898376E-4</v>
+        <v>1.3450779425656727E-4</v>
       </c>
       <c r="C158" s="215">
         <f t="shared" si="2"/>
@@ -28600,7 +28708,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>1.3996543887037646E-4</v>
+        <v>1.33467830012035E-4</v>
       </c>
       <c r="C159" s="215">
         <f t="shared" si="2"/>
@@ -28615,7 +28723,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>1.3730853781448554E-4</v>
+        <v>1.3151123282836575E-4</v>
       </c>
       <c r="C160" s="215">
         <f t="shared" si="2"/>
@@ -28630,7 +28738,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>1.3502430368333087E-4</v>
+        <v>1.2711458360919719E-4</v>
       </c>
       <c r="C161" s="215">
         <f t="shared" si="2"/>
@@ -28645,7 +28753,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>1.2915618166881306E-4</v>
+        <v>1.1960070596602893E-4</v>
       </c>
       <c r="C162" s="215">
         <f t="shared" si="2"/>
@@ -28660,7 +28768,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>1.2416608113498395E-4</v>
+        <v>1.1331136157938487E-4</v>
       </c>
       <c r="C163" s="215">
         <f t="shared" si="2"/>
@@ -28675,7 +28783,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>1.236892848004802E-4</v>
+        <v>1.0651080106319081E-4</v>
       </c>
       <c r="C164" s="215">
         <f t="shared" si="2"/>
@@ -28690,7 +28798,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>1.1004579644682239E-4</v>
+        <v>1.0268093194315097E-4</v>
       </c>
       <c r="C165" s="215">
         <f t="shared" si="2"/>
@@ -28705,7 +28813,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>1.0686869744400136E-4</v>
+        <v>8.9365112913069217E-5</v>
       </c>
       <c r="C166" s="215">
         <f t="shared" si="2"/>
@@ -28720,7 +28828,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>1.0489848001900734E-4</v>
+        <v>7.0192975731807981E-5</v>
       </c>
       <c r="C167" s="215">
         <f t="shared" si="2"/>
@@ -28735,7 +28843,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>1.0443373857403633E-4</v>
+        <v>6.6937424084161424E-5</v>
       </c>
       <c r="C168" s="215">
         <f t="shared" si="2"/>
@@ -28750,7 +28858,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>7.1963977090625574E-5</v>
+        <v>6.4427754881311701E-5</v>
       </c>
       <c r="C169" s="215">
         <f t="shared" si="2"/>
@@ -28765,7 +28873,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>7.1029331197009651E-5</v>
+        <v>6.3388025316899371E-5</v>
       </c>
       <c r="C170" s="215">
         <f t="shared" si="2"/>
@@ -28780,7 +28888,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>6.9025732300064416E-5</v>
+        <v>6.2095020684198706E-5</v>
       </c>
       <c r="C171" s="215">
         <f t="shared" si="2"/>
@@ -28795,7 +28903,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>6.6173303165213058E-5</v>
+        <v>5.9397193243992999E-5</v>
       </c>
       <c r="C172" s="215">
         <f t="shared" si="2"/>
@@ -28810,7 +28918,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>5.5899340786949375E-5</v>
+        <v>5.356010505793728E-5</v>
       </c>
       <c r="C173" s="215">
         <f t="shared" si="2"/>
@@ -28825,7 +28933,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>5.1785610338711489E-5</v>
+        <v>5.1749478908883005E-5</v>
       </c>
       <c r="C174" s="215">
         <f t="shared" si="2"/>
@@ -28840,7 +28948,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>5.1568403245883209E-5</v>
+        <v>4.8023227964161854E-5</v>
       </c>
       <c r="C175" s="215">
         <f t="shared" si="2"/>
@@ -28855,7 +28963,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>4.9573788584415942E-5</v>
+        <v>4.63298866562357E-5</v>
       </c>
       <c r="C176" s="215">
         <f t="shared" si="2"/>
@@ -28870,7 +28978,7 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>4.8646941919557083E-5</v>
+        <v>4.5385533853517606E-5</v>
       </c>
       <c r="C177" s="215">
         <f t="shared" si="2"/>
@@ -28885,7 +28993,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>4.4789283016749116E-5</v>
+        <v>4.2419922591724881E-5</v>
       </c>
       <c r="C178" s="215">
         <f t="shared" si="2"/>
@@ -28900,7 +29008,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>4.3537711182550642E-5</v>
+        <v>4.0612982301025267E-5</v>
       </c>
       <c r="C179" s="215">
         <f t="shared" si="2"/>
@@ -28915,7 +29023,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>4.1990928478682653E-5</v>
+        <v>3.9335797869352471E-5</v>
       </c>
       <c r="C180" s="215">
         <f t="shared" si="2"/>
@@ -28930,7 +29038,7 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>4.021427606369372E-5</v>
+        <v>3.4469401878302092E-5</v>
       </c>
       <c r="C181" s="215">
         <f t="shared" si="2"/>
@@ -28945,7 +29053,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>3.57033970489855E-5</v>
+        <v>3.1090367073417888E-5</v>
       </c>
       <c r="C182" s="215">
         <f t="shared" si="2"/>
@@ -28960,7 +29068,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>3.3837379770206766E-5</v>
+        <v>2.389260355183545E-5</v>
       </c>
       <c r="C183" s="215">
         <f t="shared" si="2"/>
@@ -28975,7 +29083,7 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>3.3168590878083439E-5</v>
+        <v>2.3589990439503803E-5</v>
       </c>
       <c r="C184" s="215">
         <f t="shared" si="2"/>
@@ -28990,7 +29098,7 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>2.9786196238130884E-5</v>
+        <v>2.200511276113788E-5</v>
       </c>
       <c r="C185" s="215">
         <f t="shared" si="2"/>
@@ -29005,7 +29113,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>2.9487795618432913E-5</v>
+        <v>1.4673995712566542E-5</v>
       </c>
       <c r="C186" s="215">
         <f t="shared" si="2"/>
@@ -29020,7 +29128,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>2.8565519387390181E-5</v>
+        <v>1.4291991696123799E-5</v>
       </c>
       <c r="C187" s="215">
         <f t="shared" si="2"/>
@@ -29035,7 +29143,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>2.7905045311209616E-5</v>
+        <v>1.3819580614644794E-5</v>
       </c>
       <c r="C188" s="215">
         <f t="shared" si="2"/>
@@ -29050,7 +29158,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>1.5594980626555879E-5</v>
+        <v>1.2170345364558136E-5</v>
       </c>
       <c r="C189" s="215">
         <f t="shared" si="2"/>
@@ -29065,7 +29173,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>1.5388713080254792E-5</v>
+        <v>1.2163581055218121E-5</v>
       </c>
       <c r="C190" s="215">
         <f t="shared" si="2"/>
@@ -29080,7 +29188,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>1.3863069748482871E-5</v>
+        <v>1.2038689817260709E-5</v>
       </c>
       <c r="C191" s="215">
         <f t="shared" si="2"/>
@@ -29095,7 +29203,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>1.2997503375131399E-5</v>
+        <v>9.7038434990680698E-6</v>
       </c>
       <c r="C192" s="215">
         <f t="shared" si="2"/>
@@ -29110,7 +29218,7 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>1.1391878332580339E-5</v>
+        <v>8.1843173317544709E-6</v>
       </c>
       <c r="C193" s="215">
         <f t="shared" si="2"/>
@@ -29125,7 +29233,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>8.6902776151212632E-6</v>
+        <v>7.8843823337329525E-6</v>
       </c>
       <c r="C194" s="215">
         <f t="shared" si="2"/>
@@ -29140,7 +29248,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>8.6404873402441047E-6</v>
+        <v>3.55989034909555E-6</v>
       </c>
       <c r="C195" s="215">
         <f t="shared" si="2"/>
@@ -29155,7 +29263,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>6.4933118760205351E-6</v>
+        <v>3.4667085367585843E-6</v>
       </c>
       <c r="C196" s="215">
         <f t="shared" ref="C196:C202" si="3">AVERAGE($B$2:$B$203)</f>
@@ -29170,7 +29278,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>5.8556448531297556E-6</v>
+        <v>1.1336706359609298E-6</v>
       </c>
       <c r="C197" s="215">
         <f t="shared" si="3"/>
@@ -29185,7 +29293,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>4.6376463397207115E-6</v>
+        <v>1.0780376428175266E-6</v>
       </c>
       <c r="C198" s="215">
         <f t="shared" si="3"/>
@@ -29200,7 +29308,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>1.3789169055860547E-6</v>
+        <v>3.6449964043633121E-7</v>
       </c>
       <c r="C199" s="215">
         <f t="shared" si="3"/>
@@ -29215,7 +29323,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>1.2717519723324345E-6</v>
+        <v>2.9464779296595409E-7</v>
       </c>
       <c r="C200" s="215">
         <f t="shared" si="3"/>
@@ -29230,7 +29338,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>4.8482166681834344E-7</v>
+        <v>0</v>
       </c>
       <c r="C201" s="215">
         <f t="shared" si="3"/>
@@ -29245,7 +29353,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>3.3178941186481388E-7</v>
+        <v>0</v>
       </c>
       <c r="C202" s="215">
         <f t="shared" si="3"/>
@@ -29264,7 +29372,7 @@
       </c>
       <c r="B251" s="152">
         <f>'Credit Risk Tables'!D6</f>
-        <v>0.74184585080773002</v>
+        <v>0.70595795072435885</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -29273,7 +29381,7 @@
       </c>
       <c r="B252" s="152">
         <f>'Credit Risk Tables'!D5</f>
-        <v>0.14052368340793228</v>
+        <v>0.14321007890326481</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -29282,7 +29390,7 @@
       </c>
       <c r="B253" s="152">
         <f>'Credit Risk Tables'!D7</f>
-        <v>3.6246288637051309E-2</v>
+        <v>1.6419670822658293E-2</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -29291,7 +29399,7 @@
       </c>
       <c r="B254" s="153">
         <f>'Credit Risk Tables'!D8</f>
-        <v>8.6188003814129888E-2</v>
+        <v>9.3025797079759651E-2</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="21" x14ac:dyDescent="0.35">
@@ -29300,7 +29408,7 @@
       </c>
       <c r="B255" s="1">
         <f>'Credit Risk Tables'!D10</f>
-        <v>1.0547925554549654E-3</v>
+        <v>7.1859815159926697E-4</v>
       </c>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.25">
@@ -29358,13 +29466,13 @@
         <v>117</v>
       </c>
       <c r="C282" s="84">
-        <v>0.52300000000000002</v>
+        <v>0.4824</v>
       </c>
       <c r="D282" s="84"/>
       <c r="E282" s="84"/>
       <c r="F282">
         <f>C282/42</f>
-        <v>1.2452380952380953E-2</v>
+        <v>1.1485714285714285E-2</v>
       </c>
     </row>
     <row r="283" spans="1:14" x14ac:dyDescent="0.25">
@@ -29375,13 +29483,13 @@
         <v>118</v>
       </c>
       <c r="C283" s="84">
-        <v>5.6000000000000001E-2</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="D283" s="84"/>
       <c r="E283" s="84"/>
       <c r="F283">
         <f>C283/42</f>
-        <v>1.3333333333333333E-3</v>
+        <v>1.157142857142857E-3</v>
       </c>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.25">
@@ -29392,7 +29500,7 @@
         <v>119</v>
       </c>
       <c r="C284" s="121">
-        <v>0.27200000000000002</v>
+        <v>0.32</v>
       </c>
       <c r="D284" s="84"/>
       <c r="E284" s="84"/>
@@ -30926,7 +31034,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="165">
-        <f t="shared" ref="H23:H25" si="0">G23-F23</f>
+        <f>G23-F23</f>
         <v>-1</v>
       </c>
       <c r="I23" s="160"/>
@@ -30987,7 +31095,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="165">
-        <f t="shared" si="0"/>
+        <f>G24-F24</f>
         <v>-1</v>
       </c>
       <c r="I24" s="160"/>
@@ -30998,7 +31106,7 @@
         <v>71.347687500000006</v>
       </c>
       <c r="L24" s="167">
-        <f t="shared" ref="L24:L25" si="1">J24-K24</f>
+        <f>J24-K24</f>
         <v>1.0942499999998745E-2</v>
       </c>
       <c r="M24" s="160"/>
@@ -31009,7 +31117,7 @@
         <v>100</v>
       </c>
       <c r="P24" s="167">
-        <f t="shared" ref="P24:P25" si="2">N24-O24</f>
+        <f>N24-O24</f>
         <v>0</v>
       </c>
       <c r="Q24" s="168"/>
@@ -31020,7 +31128,7 @@
         <v>90.26</v>
       </c>
       <c r="T24" s="167">
-        <f t="shared" ref="T24:T25" si="3">R24-S24</f>
+        <f>R24-S24</f>
         <v>-20.897654192178209</v>
       </c>
       <c r="U24" s="183" t="s">
@@ -31048,7 +31156,7 @@
         <v>3</v>
       </c>
       <c r="H25" s="165">
-        <f t="shared" si="0"/>
+        <f>G25-F25</f>
         <v>-1</v>
       </c>
       <c r="I25" s="160"/>
@@ -31059,7 +31167,7 @@
         <v>40.500644999999999</v>
       </c>
       <c r="L25" s="167">
-        <f t="shared" si="1"/>
+        <f>J25-K25</f>
         <v>0.59870624999999933</v>
       </c>
       <c r="M25" s="160"/>
@@ -31070,7 +31178,7 @@
         <v>100</v>
       </c>
       <c r="P25" s="167">
-        <f t="shared" si="2"/>
+        <f>N25-O25</f>
         <v>-1.8205790084436586</v>
       </c>
       <c r="Q25" s="168"/>
@@ -31081,7 +31189,7 @@
         <v>0</v>
       </c>
       <c r="T25" s="167">
-        <f t="shared" si="3"/>
+        <f>R25-S25</f>
         <v>0</v>
       </c>
       <c r="U25" s="218" t="s">
@@ -31286,7 +31394,7 @@
         <v>4</v>
       </c>
       <c r="H32" s="165">
-        <f t="shared" ref="H32:H35" si="4">G32-F32</f>
+        <f>G32-F32</f>
         <v>2</v>
       </c>
       <c r="I32" s="160"/>
@@ -31345,7 +31453,7 @@
         <v>4</v>
       </c>
       <c r="H33" s="165">
-        <f t="shared" si="4"/>
+        <f>G33-F33</f>
         <v>1</v>
       </c>
       <c r="I33" s="160"/>
@@ -31356,7 +31464,7 @@
         <v>50.39733167</v>
       </c>
       <c r="L33" s="167">
-        <f t="shared" ref="L33:L35" si="5">J33-K33</f>
+        <f>J33-K33</f>
         <v>1.1110000000002174E-2</v>
       </c>
       <c r="M33" s="160"/>
@@ -31367,7 +31475,7 @@
         <v>100</v>
       </c>
       <c r="P33" s="167">
-        <f t="shared" ref="P33:P35" si="6">N33-O33</f>
+        <f>N33-O33</f>
         <v>0</v>
       </c>
       <c r="Q33" s="168"/>
@@ -31378,7 +31486,7 @@
         <v>0</v>
       </c>
       <c r="T33" s="167">
-        <f t="shared" ref="T33:T35" si="7">R33-S33</f>
+        <f>R33-S33</f>
         <v>0</v>
       </c>
       <c r="U33" s="167"/>
@@ -31404,7 +31512,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="165">
-        <f t="shared" si="4"/>
+        <f>G34-F34</f>
         <v>2</v>
       </c>
       <c r="I34" s="160"/>
@@ -31415,7 +31523,7 @@
         <v>68.382322500000001</v>
       </c>
       <c r="L34" s="167">
-        <f t="shared" si="5"/>
+        <f>J34-K34</f>
         <v>-0.1250725000000017</v>
       </c>
       <c r="M34" s="160"/>
@@ -31426,7 +31534,7 @@
         <v>100</v>
       </c>
       <c r="P34" s="167">
-        <f t="shared" si="6"/>
+        <f>N34-O34</f>
         <v>0</v>
       </c>
       <c r="Q34" s="168"/>
@@ -31437,7 +31545,7 @@
         <v>50.508867408877876</v>
       </c>
       <c r="T34" s="167">
-        <f t="shared" si="7"/>
+        <f>R34-S34</f>
         <v>-11.799524957749739</v>
       </c>
       <c r="U34" s="167"/>
@@ -31463,7 +31571,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="165">
-        <f t="shared" si="4"/>
+        <f>G35-F35</f>
         <v>1</v>
       </c>
       <c r="I35" s="160"/>
@@ -31474,7 +31582,7 @@
         <v>79.303558330000001</v>
       </c>
       <c r="L35" s="167">
-        <f t="shared" si="5"/>
+        <f>J35-K35</f>
         <v>2.6336669999992068E-2</v>
       </c>
       <c r="M35" s="160"/>
@@ -31485,7 +31593,7 @@
         <v>100</v>
       </c>
       <c r="P35" s="167">
-        <f t="shared" si="6"/>
+        <f>N35-O35</f>
         <v>0</v>
       </c>
       <c r="Q35" s="168"/>
@@ -31496,7 +31604,7 @@
         <v>93.438451538461194</v>
       </c>
       <c r="T35" s="167">
-        <f t="shared" si="7"/>
+        <f>R35-S35</f>
         <v>6.5615484615388056</v>
       </c>
       <c r="U35" s="167"/>
@@ -31687,14 +31795,14 @@
         <v>0.6936234580782179</v>
       </c>
       <c r="I45" s="122">
-        <f t="shared" ref="I45:I46" si="8">H45*100</f>
+        <f>H45*100</f>
         <v>69.362345807821796</v>
       </c>
       <c r="K45" s="122">
         <v>0</v>
       </c>
       <c r="L45" s="122">
-        <f t="shared" ref="L45:L47" si="9">K45*100</f>
+        <f>K45*100</f>
         <v>0</v>
       </c>
     </row>
@@ -31703,14 +31811,14 @@
         <v>0</v>
       </c>
       <c r="I46" s="122">
-        <f t="shared" si="8"/>
+        <f>H46*100</f>
         <v>0</v>
       </c>
       <c r="K46" s="122">
         <v>0.38709342451128137</v>
       </c>
       <c r="L46" s="122">
-        <f t="shared" si="9"/>
+        <f>K46*100</f>
         <v>38.709342451128137</v>
       </c>
     </row>
@@ -31719,7 +31827,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="122">
-        <f t="shared" si="9"/>
+        <f>K47*100</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>